<commit_message>
Fixed up the power calculation to show on the display, accuracy is around 3%
</commit_message>
<xml_diff>
--- a/Firmware/EnergyMonitor/analysis.xlsx
+++ b/Firmware/EnergyMonitor/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y3J5bw\ownCloud\UoA\2024\Semester 2 2024\COMPSYS 209\ec209-project-2024_team_33\Firmware\EnergyMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5781388-1735-445B-ACB7-7EE5B11F8B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06ECC5E-C961-4044-AAB7-05FD718C52C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="26136" xr2:uid="{5B712931-4F47-4E8C-8387-F250B08A1400}"/>
   </bookViews>
@@ -2834,10 +2834,13 @@
   <dimension ref="E8:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:F61"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="26" max="27" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="8" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E8">

</xml_diff>

<commit_message>
Fixed the phase calculation, error is now around 1.5% now
</commit_message>
<xml_diff>
--- a/Firmware/EnergyMonitor/analysis.xlsx
+++ b/Firmware/EnergyMonitor/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y3J5bw\ownCloud\UoA\2024\Semester 2 2024\COMPSYS 209\ec209-project-2024_team_33\Firmware\EnergyMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06ECC5E-C961-4044-AAB7-05FD718C52C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9637A2-B881-47FD-A6BC-BF13C1DD2E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="26136" xr2:uid="{5B712931-4F47-4E8C-8387-F250B08A1400}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Phase</t>
   </si>
@@ -57,6 +57,48 @@
   </si>
   <si>
     <t>RMS Current: 2749 mA</t>
+  </si>
+  <si>
+    <t>RMS Current: 1435 mA</t>
+  </si>
+  <si>
+    <t>RMS Voltage: 2033 mV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Power: 2489 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phase: 548 </t>
+  </si>
+  <si>
+    <t>RMS Voltage: 2029 mV</t>
+  </si>
+  <si>
+    <t>RMS Current: 1431 mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Power: 2482 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phase: 545 </t>
+  </si>
+  <si>
+    <t>RMS Voltage: 2031 mV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Power: 2806 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phase: 262 </t>
+  </si>
+  <si>
+    <t>RMS Voltage: 2041 mV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Power: 2483 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phase: 554 </t>
   </si>
 </sst>
 </file>
@@ -1351,6 +1393,665 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$40:$Q$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>837</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>647</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>905</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>893</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>393</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>899</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>857</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3472</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>759</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>904</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CEA3-4949-A591-2559CCC2177A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$40:$R$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>697</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>652</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>538</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>614</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>709</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43994</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CEA3-4949-A591-2559CCC2177A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="106508096"/>
+        <c:axId val="106502816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="106508096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="106502816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="106502816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="106508096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1431,6 +2132,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1935,6 +2676,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2506,6 +3750,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECFCA800-10E0-7D97-71FE-B22611C8BD76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2831,10 +4111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88EF616-250D-46CA-B716-E8A9B416F08C}">
-  <dimension ref="E8:R61"/>
+  <dimension ref="E8:R247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38:R247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3454,7 +4734,7 @@
         <v>1.97265625</v>
       </c>
     </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E33">
         <v>919</v>
       </c>
@@ -3478,7 +4758,7 @@
         <v>1.416015625</v>
       </c>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E34">
         <v>855</v>
       </c>
@@ -3502,7 +4782,7 @@
         <v>0.322265625</v>
       </c>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>660</v>
       </c>
@@ -3526,7 +4806,7 @@
         <v>-0.8984375</v>
       </c>
     </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E36">
         <v>408</v>
       </c>
@@ -3550,7 +4830,7 @@
         <v>-1.77734375</v>
       </c>
     </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>195</v>
       </c>
@@ -3574,7 +4854,7 @@
         <v>-1.962890625</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>103</v>
       </c>
@@ -3597,8 +4877,14 @@
         <f t="shared" si="7"/>
         <v>-1.416015625</v>
       </c>
-    </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q38">
+        <v>3490</v>
+      </c>
+      <c r="R38">
+        <v>43995</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>168</v>
       </c>
@@ -3621,8 +4907,11 @@
         <f t="shared" si="7"/>
         <v>-0.322265625</v>
       </c>
-    </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q39">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E40">
         <v>364</v>
       </c>
@@ -3645,8 +4934,14 @@
         <f t="shared" si="7"/>
         <v>0.8984375</v>
       </c>
-    </row>
-    <row r="41" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q40">
+        <v>403</v>
+      </c>
+      <c r="R40">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="41" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E41">
         <v>616</v>
       </c>
@@ -3669,8 +4964,14 @@
         <f t="shared" si="7"/>
         <v>1.77734375</v>
       </c>
-    </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q41">
+        <v>760</v>
+      </c>
+      <c r="R41">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="42" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E42">
         <v>827</v>
       </c>
@@ -3693,8 +4994,14 @@
         <f t="shared" si="7"/>
         <v>1.97265625</v>
       </c>
-    </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q42">
+        <v>903</v>
+      </c>
+      <c r="R42">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E43">
         <v>919</v>
       </c>
@@ -3717,8 +5024,14 @@
         <f t="shared" si="7"/>
         <v>1.416015625</v>
       </c>
-    </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q43">
+        <v>896</v>
+      </c>
+      <c r="R43">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="44" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E44">
         <v>855</v>
       </c>
@@ -3741,8 +5054,14 @@
         <f t="shared" si="7"/>
         <v>0.322265625</v>
       </c>
-    </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q44">
+        <v>744</v>
+      </c>
+      <c r="R44">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="45" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E45">
         <v>660</v>
       </c>
@@ -3765,8 +5084,14 @@
         <f t="shared" si="7"/>
         <v>-0.8984375</v>
       </c>
-    </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q45">
+        <v>502</v>
+      </c>
+      <c r="R45">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E46">
         <v>408</v>
       </c>
@@ -3789,8 +5114,14 @@
         <f t="shared" si="7"/>
         <v>-1.77734375</v>
       </c>
-    </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q46">
+        <v>263</v>
+      </c>
+      <c r="R46">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="47" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E47">
         <v>195</v>
       </c>
@@ -3813,8 +5144,14 @@
         <f t="shared" si="7"/>
         <v>-1.962890625</v>
       </c>
-    </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q47">
+        <v>120</v>
+      </c>
+      <c r="R47">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E48">
         <v>103</v>
       </c>
@@ -3837,8 +5174,14 @@
         <f t="shared" si="7"/>
         <v>-1.416015625</v>
       </c>
-    </row>
-    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q48">
+        <v>127</v>
+      </c>
+      <c r="R48">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="49" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E49">
         <v>168</v>
       </c>
@@ -3861,8 +5204,14 @@
         <f t="shared" si="7"/>
         <v>-0.322265625</v>
       </c>
-    </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q49">
+        <v>280</v>
+      </c>
+      <c r="R49">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="50" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E50">
         <v>364</v>
       </c>
@@ -3885,8 +5234,14 @@
         <f t="shared" si="7"/>
         <v>0.8984375</v>
       </c>
-    </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q50">
+        <v>504</v>
+      </c>
+      <c r="R50">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="51" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E51">
         <v>616</v>
       </c>
@@ -3909,8 +5264,14 @@
         <f t="shared" si="7"/>
         <v>1.77734375</v>
       </c>
-    </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q51">
+        <v>837</v>
+      </c>
+      <c r="R51">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="52" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E52">
         <v>829</v>
       </c>
@@ -3933,8 +5294,14 @@
         <f t="shared" ref="L52:L54" si="11">(I52-2.5)*2</f>
         <v>1.962890625</v>
       </c>
-    </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q52">
+        <v>920</v>
+      </c>
+      <c r="R52">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="53" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E53">
         <v>920</v>
       </c>
@@ -3957,8 +5324,14 @@
         <f t="shared" si="11"/>
         <v>1.416015625</v>
       </c>
-    </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q53">
+        <v>847</v>
+      </c>
+      <c r="R53">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="54" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E54">
         <v>856</v>
       </c>
@@ -3981,8 +5354,14 @@
         <f t="shared" si="11"/>
         <v>0.322265625</v>
       </c>
-    </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q54">
+        <v>647</v>
+      </c>
+      <c r="R54">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="55" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E55">
         <v>660</v>
       </c>
@@ -4005,8 +5384,14 @@
         <f t="shared" ref="L55:L56" si="13">(I55-2.5)*2</f>
         <v>-0.8984375</v>
       </c>
-    </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q55">
+        <v>394</v>
+      </c>
+      <c r="R55">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="56" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E56">
         <v>408</v>
       </c>
@@ -4029,39 +5414,1506 @@
         <f t="shared" si="13"/>
         <v>-1.77734375</v>
       </c>
-    </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q56">
+        <v>186</v>
+      </c>
+      <c r="R56">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="57" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E57">
         <v>195</v>
       </c>
       <c r="F57">
         <v>311</v>
       </c>
-    </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q57">
+        <v>104</v>
+      </c>
+      <c r="R57">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="58" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E58">
         <v>103</v>
       </c>
       <c r="F58">
         <v>367</v>
       </c>
-    </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q58">
+        <v>176</v>
+      </c>
+      <c r="R58">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="59" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E59">
         <v>168</v>
       </c>
       <c r="F59">
         <v>479</v>
       </c>
-    </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q59">
+        <v>411</v>
+      </c>
+      <c r="R59">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="60" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="Q60">
+        <v>767</v>
+      </c>
+      <c r="R60">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="61" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E61" t="s">
         <v>6</v>
+      </c>
+      <c r="Q61">
+        <v>905</v>
+      </c>
+      <c r="R61">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="62" spans="5:18" x14ac:dyDescent="0.3">
+      <c r="Q62">
+        <v>893</v>
+      </c>
+      <c r="R62">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="63" spans="5:18" x14ac:dyDescent="0.3">
+      <c r="Q63">
+        <v>737</v>
+      </c>
+      <c r="R63">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="64" spans="5:18" x14ac:dyDescent="0.3">
+      <c r="Q64">
+        <v>493</v>
+      </c>
+      <c r="R64">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="65" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q65">
+        <v>257</v>
+      </c>
+      <c r="R65">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="66" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q66">
+        <v>117</v>
+      </c>
+      <c r="R66">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="67" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q67">
+        <v>129</v>
+      </c>
+      <c r="R67">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="68" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q68">
+        <v>393</v>
+      </c>
+      <c r="R68">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="69" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q69">
+        <v>752</v>
+      </c>
+      <c r="R69">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="70" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q70">
+        <v>899</v>
+      </c>
+      <c r="R70">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="71" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q71">
+        <v>900</v>
+      </c>
+      <c r="R71">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="72" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q72">
+        <v>752</v>
+      </c>
+      <c r="R72">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="73" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q73">
+        <v>512</v>
+      </c>
+      <c r="R73">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="74" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q74">
+        <v>271</v>
+      </c>
+      <c r="R74">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="75" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q75">
+        <v>124</v>
+      </c>
+      <c r="R75">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="76" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q76">
+        <v>124</v>
+      </c>
+      <c r="R76">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="77" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q77">
+        <v>271</v>
+      </c>
+      <c r="R77">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="78" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q78">
+        <v>664</v>
+      </c>
+      <c r="R78">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="79" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q79">
+        <v>857</v>
+      </c>
+      <c r="R79">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="80" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q80">
+        <v>918</v>
+      </c>
+      <c r="R80">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="81" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q81">
+        <v>825</v>
+      </c>
+      <c r="R81">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="82" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q82">
+        <v>612</v>
+      </c>
+      <c r="R82">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="83" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q83">
+        <v>360</v>
+      </c>
+      <c r="R83">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="84" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q84">
+        <v>166</v>
+      </c>
+      <c r="R84">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="85" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q85">
+        <v>103</v>
+      </c>
+      <c r="R85">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="86" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q90">
+        <v>3472</v>
+      </c>
+      <c r="R90">
+        <v>43994</v>
+      </c>
+    </row>
+    <row r="91" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q91">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q92">
+        <v>562</v>
+      </c>
+      <c r="R92">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="93" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q93">
+        <v>759</v>
+      </c>
+      <c r="R93">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="94" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q94">
+        <v>904</v>
+      </c>
+      <c r="R94">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="95" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q95">
+        <v>899</v>
+      </c>
+      <c r="R95">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="96" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q96">
+        <v>746</v>
+      </c>
+      <c r="R96">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="97" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q97">
+        <v>504</v>
+      </c>
+      <c r="R97">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="98" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q98">
+        <v>265</v>
+      </c>
+      <c r="R98">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="99" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q99">
+        <v>121</v>
+      </c>
+      <c r="R99">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="100" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q100">
+        <v>126</v>
+      </c>
+      <c r="R100">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="101" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q101">
+        <v>278</v>
+      </c>
+      <c r="R101">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="102" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q102">
+        <v>502</v>
+      </c>
+      <c r="R102">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="103" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q103">
+        <v>836</v>
+      </c>
+      <c r="R103">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="104" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q104">
+        <v>921</v>
+      </c>
+      <c r="R104">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="105" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q105">
+        <v>847</v>
+      </c>
+      <c r="R105">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="106" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q106">
+        <v>648</v>
+      </c>
+      <c r="R106">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="107" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q107">
+        <v>395</v>
+      </c>
+      <c r="R107">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="108" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q108">
+        <v>186</v>
+      </c>
+      <c r="R108">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="109" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q109">
+        <v>105</v>
+      </c>
+      <c r="R109">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="110" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q110">
+        <v>177</v>
+      </c>
+      <c r="R110">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="111" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q111">
+        <v>409</v>
+      </c>
+      <c r="R111">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="112" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q112">
+        <v>765</v>
+      </c>
+      <c r="R112">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="113" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q113">
+        <v>904</v>
+      </c>
+      <c r="R113">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="114" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q114">
+        <v>894</v>
+      </c>
+      <c r="R114">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="115" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q115">
+        <v>738</v>
+      </c>
+      <c r="R115">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="116" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q116">
+        <v>495</v>
+      </c>
+      <c r="R116">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="117" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q117">
+        <v>258</v>
+      </c>
+      <c r="R117">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="118" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q118">
+        <v>118</v>
+      </c>
+      <c r="R118">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="119" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q119">
+        <v>128</v>
+      </c>
+      <c r="R119">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="120" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q120">
+        <v>285</v>
+      </c>
+      <c r="R120">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="121" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q121">
+        <v>509</v>
+      </c>
+      <c r="R121">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="122" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q122">
+        <v>841</v>
+      </c>
+      <c r="R122">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="123" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q123">
+        <v>922</v>
+      </c>
+      <c r="R123">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="124" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q124">
+        <v>845</v>
+      </c>
+      <c r="R124">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="125" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q125">
+        <v>641</v>
+      </c>
+      <c r="R125">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="126" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q126">
+        <v>389</v>
+      </c>
+      <c r="R126">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="127" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q127">
+        <v>182</v>
+      </c>
+      <c r="R127">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="128" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q128">
+        <v>102</v>
+      </c>
+      <c r="R128">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="129" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q129">
+        <v>179</v>
+      </c>
+      <c r="R129">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="130" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q130">
+        <v>416</v>
+      </c>
+      <c r="R130">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="131" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q131">
+        <v>772</v>
+      </c>
+      <c r="R131">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="132" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q132">
+        <v>906</v>
+      </c>
+      <c r="R132">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="133" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q133">
+        <v>891</v>
+      </c>
+      <c r="R133">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="134" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q134">
+        <v>733</v>
+      </c>
+      <c r="R134">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="135" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q135">
+        <v>488</v>
+      </c>
+      <c r="R135">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="136" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q136">
+        <v>253</v>
+      </c>
+      <c r="R136">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="137" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q137">
+        <v>116</v>
+      </c>
+      <c r="R137">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="138" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q138">
+        <v>131</v>
+      </c>
+      <c r="R138">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="139" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q139" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q140" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="141" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q141" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="142" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q142" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q143">
+        <v>1670</v>
+      </c>
+      <c r="R143">
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="144" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q144">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="145" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q145">
+        <v>398</v>
+      </c>
+      <c r="R145">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="146" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q146">
+        <v>756</v>
+      </c>
+      <c r="R146">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="147" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q147">
+        <v>901</v>
+      </c>
+      <c r="R147">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="148" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q148">
+        <v>900</v>
+      </c>
+      <c r="R148">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="149" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q149">
+        <v>748</v>
+      </c>
+      <c r="R149">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="150" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q150">
+        <v>507</v>
+      </c>
+      <c r="R150">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="151" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q151">
+        <v>267</v>
+      </c>
+      <c r="R151">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="152" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q152">
+        <v>121</v>
+      </c>
+      <c r="R152">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="153" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q153">
+        <v>126</v>
+      </c>
+      <c r="R153">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="154" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q154">
+        <v>276</v>
+      </c>
+      <c r="R154">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="155" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q155">
+        <v>498</v>
+      </c>
+      <c r="R155">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="156" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q156">
+        <v>834</v>
+      </c>
+      <c r="R156">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="157" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q157">
+        <v>921</v>
+      </c>
+      <c r="R157">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="158" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q158">
+        <v>851</v>
+      </c>
+      <c r="R158">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="159" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q159">
+        <v>651</v>
+      </c>
+      <c r="R159">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="160" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q160">
+        <v>398</v>
+      </c>
+      <c r="R160">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="161" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q161">
+        <v>191</v>
+      </c>
+      <c r="R161">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="162" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q162">
+        <v>104</v>
+      </c>
+      <c r="R162">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="163" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q163">
+        <v>175</v>
+      </c>
+      <c r="R163">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="164" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q164">
+        <v>407</v>
+      </c>
+      <c r="R164">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="165" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q165">
+        <v>763</v>
+      </c>
+      <c r="R165">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="166" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q166">
+        <v>906</v>
+      </c>
+      <c r="R166">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="167" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q167">
+        <v>897</v>
+      </c>
+      <c r="R167">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="168" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q168">
+        <v>741</v>
+      </c>
+      <c r="R168">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="169" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q169">
+        <v>498</v>
+      </c>
+      <c r="R169">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="170" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q170">
+        <v>260</v>
+      </c>
+      <c r="R170">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="171" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q171">
+        <v>119</v>
+      </c>
+      <c r="R171">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="172" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q172">
+        <v>128</v>
+      </c>
+      <c r="R172">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="173" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q173">
+        <v>284</v>
+      </c>
+      <c r="R173">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="174" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q174">
+        <v>507</v>
+      </c>
+      <c r="R174">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="175" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q175">
+        <v>840</v>
+      </c>
+      <c r="R175">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="176" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q176">
+        <v>920</v>
+      </c>
+      <c r="R176">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="177" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q177">
+        <v>846</v>
+      </c>
+      <c r="R177">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="178" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q178">
+        <v>643</v>
+      </c>
+      <c r="R178">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="179" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q179">
+        <v>390</v>
+      </c>
+      <c r="R179">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="180" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q180">
+        <v>183</v>
+      </c>
+      <c r="R180">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="181" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q181">
+        <v>102</v>
+      </c>
+      <c r="R181">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="182" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q182">
+        <v>178</v>
+      </c>
+      <c r="R182">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="183" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q183">
+        <v>415</v>
+      </c>
+      <c r="R183">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="184" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q184">
+        <v>771</v>
+      </c>
+      <c r="R184">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="185" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q185">
+        <v>906</v>
+      </c>
+      <c r="R185">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="186" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q186">
+        <v>892</v>
+      </c>
+      <c r="R186">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="187" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q187">
+        <v>734</v>
+      </c>
+      <c r="R187">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="188" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q188">
+        <v>489</v>
+      </c>
+      <c r="R188">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="189" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q189">
+        <v>254</v>
+      </c>
+      <c r="R189">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="190" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q190">
+        <v>116</v>
+      </c>
+      <c r="R190">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="191" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q191">
+        <v>132</v>
+      </c>
+      <c r="R191">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="192" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q192" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="193" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q193" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="194" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q194" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="195" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q195" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="196" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q196">
+        <v>3529</v>
+      </c>
+      <c r="R196">
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="197" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q197">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="198" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q198">
+        <v>397</v>
+      </c>
+      <c r="R198">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="199" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q199">
+        <v>756</v>
+      </c>
+      <c r="R199">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="200" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q200">
+        <v>903</v>
+      </c>
+      <c r="R200">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="201" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q201">
+        <v>898</v>
+      </c>
+      <c r="R201">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="202" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q202">
+        <v>748</v>
+      </c>
+      <c r="R202">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="203" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q203">
+        <v>508</v>
+      </c>
+      <c r="R203">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="204" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q204">
+        <v>268</v>
+      </c>
+      <c r="R204">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="205" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q205">
+        <v>123</v>
+      </c>
+      <c r="R205">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="206" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q206">
+        <v>125</v>
+      </c>
+      <c r="R206">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="207" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q207">
+        <v>275</v>
+      </c>
+      <c r="R207">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="208" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q208">
+        <v>667</v>
+      </c>
+      <c r="R208">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="209" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q209">
+        <v>861</v>
+      </c>
+      <c r="R209">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="210" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q210">
+        <v>918</v>
+      </c>
+      <c r="R210">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="211" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q211">
+        <v>823</v>
+      </c>
+      <c r="R211">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="212" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q212">
+        <v>609</v>
+      </c>
+      <c r="R212">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="213" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q213">
+        <v>356</v>
+      </c>
+      <c r="R213">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="214" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q214">
+        <v>164</v>
+      </c>
+      <c r="R214">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="215" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q215">
+        <v>105</v>
+      </c>
+      <c r="R215">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="216" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q216">
+        <v>200</v>
+      </c>
+      <c r="R216">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="217" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q217">
+        <v>524</v>
+      </c>
+      <c r="R217">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="218" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q218">
+        <v>850</v>
+      </c>
+      <c r="R218">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="219" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q219">
+        <v>919</v>
+      </c>
+      <c r="R219">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="220" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q220">
+        <v>834</v>
+      </c>
+      <c r="R220">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="221" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q221">
+        <v>627</v>
+      </c>
+      <c r="R221">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="222" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q222">
+        <v>374</v>
+      </c>
+      <c r="R222">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="223" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q223">
+        <v>174</v>
+      </c>
+      <c r="R223">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="224" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q224">
+        <v>103</v>
+      </c>
+      <c r="R224">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="225" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q225">
+        <v>188</v>
+      </c>
+      <c r="R225">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="226" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q226">
+        <v>386</v>
+      </c>
+      <c r="R226">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="227" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q227">
+        <v>747</v>
+      </c>
+      <c r="R227">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="228" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q228">
+        <v>899</v>
+      </c>
+      <c r="R228">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="229" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q229">
+        <v>904</v>
+      </c>
+      <c r="R229">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="230" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q230">
+        <v>757</v>
+      </c>
+      <c r="R230">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="231" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q231">
+        <v>519</v>
+      </c>
+      <c r="R231">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="232" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q232">
+        <v>277</v>
+      </c>
+      <c r="R232">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="233" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q233">
+        <v>127</v>
+      </c>
+      <c r="R233">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="234" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q234">
+        <v>122</v>
+      </c>
+      <c r="R234">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="235" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q235">
+        <v>266</v>
+      </c>
+      <c r="R235">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="236" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q236">
+        <v>658</v>
+      </c>
+      <c r="R236">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="237" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q237">
+        <v>854</v>
+      </c>
+      <c r="R237">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="238" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q238">
+        <v>920</v>
+      </c>
+      <c r="R238">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="239" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q239">
+        <v>830</v>
+      </c>
+      <c r="R239">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="240" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q240">
+        <v>619</v>
+      </c>
+      <c r="R240">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="241" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q241">
+        <v>366</v>
+      </c>
+      <c r="R241">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="242" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q242">
+        <v>170</v>
+      </c>
+      <c r="R242">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="243" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q243">
+        <v>105</v>
+      </c>
+      <c r="R243">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="244" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q244" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="245" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q245" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="246" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q246" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="247" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q247" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working power calculation and everything now, inaccuracies at extreme values of Rload otherwise errir is around 1.25%
</commit_message>
<xml_diff>
--- a/Firmware/EnergyMonitor/analysis.xlsx
+++ b/Firmware/EnergyMonitor/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y3J5bw\ownCloud\UoA\2024\Semester 2 2024\COMPSYS 209\ec209-project-2024_team_33\Firmware\EnergyMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ECE6F9-8BF6-4CA0-B371-822D3221F8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE75C808-B303-432F-9A45-6FB5C072032C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="26136" activeTab="1" xr2:uid="{5B712931-4F47-4E8C-8387-F250B08A1400}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -4760,40 +4760,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.8174896250334376</c:v>
+                  <c:v>2.5427284635984018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1508655032779052</c:v>
+                  <c:v>2.6925214866721121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.235632881375019</c:v>
+                  <c:v>2.7687778454017353</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.039413502028895</c:v>
+                  <c:v>2.7423702026108603</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6371564988983436</c:v>
+                  <c:v>2.6233853802828349</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1825103749665624</c:v>
+                  <c:v>2.4572715364015982</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8491344967220948</c:v>
+                  <c:v>2.3074785133278879</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.764367118624981</c:v>
+                  <c:v>2.2312221545982647</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9605864979711052</c:v>
+                  <c:v>2.2576297973891402</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3628435011016564</c:v>
+                  <c:v>2.3766146197171651</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8174896250334376</c:v>
+                  <c:v>2.5427284635984022</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.1508655032779052</c:v>
+                  <c:v>2.6925214866721121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11426,8 +11426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A733CF-01AB-433F-B8EB-89FAB0430329}">
   <dimension ref="B3:AD137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="AB29" sqref="AB29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11463,24 +11463,24 @@
         <v>12.566370614359172</v>
       </c>
       <c r="D5">
-        <f>26.25+0.282</f>
-        <v>26.532</v>
+        <f>105*0.75+0.282</f>
+        <v>79.031999999999996</v>
       </c>
       <c r="E5">
         <f>SQRT(SUMSQ(C5:D5))</f>
-        <v>29.357464032464211</v>
+        <v>80.024812992080328</v>
       </c>
       <c r="F5">
         <f>14/E5</f>
-        <v>0.47688042756412657</v>
+        <v>0.17494573840972941</v>
       </c>
       <c r="G5">
         <f>F5*0.282*SQRT(2)</f>
-        <v>0.19018383665819399</v>
+        <v>6.9769799334633037E-2</v>
       </c>
       <c r="H5">
         <f>ATAN(C5/D5)</f>
-        <v>0.44233054492406659</v>
+        <v>0.1576835591301893</v>
       </c>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.3">
@@ -11517,7 +11517,7 @@
       </c>
       <c r="E10">
         <f>G5*SIN(C10+H5)</f>
-        <v>8.1407596162419896E-2</v>
+        <v>1.0956016307282553E-2</v>
       </c>
       <c r="G10">
         <f>D10*E10/0.282</f>
@@ -11525,7 +11525,7 @@
       </c>
       <c r="J10">
         <f>AVERAGE(G11:G32)</f>
-        <v>6.123007355011012</v>
+        <v>2.4074217603139245</v>
       </c>
       <c r="L10">
         <f>SQRT(SUMSQ(D11:D32)/COUNT(D11:D32))</f>
@@ -11533,15 +11533,15 @@
       </c>
       <c r="M10">
         <f>SQRT(SUMSQ(E11:E32)/COUNT(E11:E32))/0.282</f>
-        <v>0.48361361558757843</v>
+        <v>0.17518358748029594</v>
       </c>
       <c r="N10">
         <f>L10*M10*COS(H5)</f>
-        <v>6.0784983997987005</v>
+        <v>2.4061242845532713</v>
       </c>
       <c r="P10">
         <f>14*F5*COS(H5)</f>
-        <v>6.0337732462844205</v>
+        <v>2.4188542919947187</v>
       </c>
       <c r="R10">
         <f>D10/23+2.5</f>
@@ -11549,7 +11549,7 @@
       </c>
       <c r="S10">
         <f>E10*3.9+2.5</f>
-        <v>2.8174896250334376</v>
+        <v>2.5427284635984018</v>
       </c>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.3">
@@ -11563,18 +11563,18 @@
       </c>
       <c r="E11">
         <f>G5*SIN(C11+H5)</f>
-        <v>0.16688859058407823</v>
+        <v>4.936448376207999E-2</v>
       </c>
       <c r="G11">
         <f>D11*E11/0.282</f>
-        <v>6.8871454890948822</v>
+        <v>2.0371697098863395</v>
       </c>
       <c r="I11" t="s">
         <v>25</v>
       </c>
       <c r="J11">
         <f>(J10-P10)/P10*100</f>
-        <v>1.478910543771953</v>
+        <v>-0.47264242904711218</v>
       </c>
       <c r="L11">
         <f>(L10-14)/L10*100</f>
@@ -11582,19 +11582,23 @@
       </c>
       <c r="M11">
         <f>(M10-F5)/F5*100</f>
-        <v>1.411923751587904</v>
+        <v>0.13595590994590886</v>
       </c>
       <c r="N11">
         <f>(N10-P10)/P10*100</f>
-        <v>0.74124683989113604</v>
+        <v>-0.52628252489526806</v>
+      </c>
+      <c r="P11">
+        <f>(2.38-P10)/P10*100</f>
+        <v>-1.6063097361138454</v>
       </c>
       <c r="R11">
-        <f t="shared" ref="R11:S32" si="0">D11/23+2.5</f>
+        <f t="shared" ref="R11:R32" si="0">D11/23+2.5</f>
         <v>3.0059806199029868</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S32" si="1">E11*3.9+2.5</f>
-        <v>3.1508655032779052</v>
+        <v>2.6925214866721121</v>
       </c>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.3">
@@ -11608,11 +11612,11 @@
       </c>
       <c r="E12">
         <f>G5*SIN(C12+H5)</f>
-        <v>0.18862381573718434</v>
+        <v>6.8917396256855154E-2</v>
       </c>
       <c r="G12">
         <f t="shared" ref="G12:G32" si="3">D12*E12/0.282</f>
-        <v>12.594959543681432</v>
+        <v>4.6018145392646588</v>
       </c>
       <c r="R12">
         <f t="shared" si="0"/>
@@ -11620,7 +11624,7 @@
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>3.235632881375019</v>
+        <v>2.7687778454017353</v>
       </c>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.3">
@@ -11634,11 +11638,11 @@
       </c>
       <c r="E13">
         <f>G5*SIN(C13+H5)</f>
-        <v>0.13831115436638336</v>
+        <v>6.2146205797656437E-2</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>9.2354371417853915</v>
+        <v>4.1496825030057982</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
@@ -11646,7 +11650,7 @@
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>3.039413502028895</v>
+        <v>2.7423702026108603</v>
       </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.3">
@@ -11660,11 +11664,11 @@
       </c>
       <c r="E14">
         <f>G5*SIN(C14+H5)</f>
-        <v>3.5168333050857363E-2</v>
+        <v>3.1637276995598727E-2</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>1.4513240568604</v>
+        <v>1.3056047078168003</v>
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
@@ -11672,7 +11676,7 @@
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>2.6371564988983436</v>
+        <v>2.6233853802828349</v>
       </c>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.3">
@@ -11686,11 +11690,11 @@
       </c>
       <c r="E15">
         <f>G5*SIN(C15+H5)</f>
-        <v>-8.1407596162419854E-2</v>
+        <v>-1.095601630728254E-2</v>
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>-7.0024105978518403E-16</v>
+        <v>-9.4240007464768242E-17</v>
       </c>
       <c r="R15">
         <f t="shared" si="0"/>
@@ -11698,7 +11702,7 @@
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>2.1825103749665624</v>
+        <v>2.4572715364015982</v>
       </c>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.3">
@@ -11712,11 +11716,11 @@
       </c>
       <c r="E16">
         <f>G5*SIN(C16+H5)</f>
-        <v>-0.16688859058407823</v>
+        <v>-4.936448376207999E-2</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>6.8871454890948796</v>
+        <v>2.0371697098863391</v>
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
@@ -11724,7 +11728,7 @@
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>1.8491344967220948</v>
+        <v>2.3074785133278879</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
@@ -11738,11 +11742,11 @@
       </c>
       <c r="E17">
         <f>G5*SIN(C17+H5)</f>
-        <v>-0.18862381573718434</v>
+        <v>-6.8917396256855168E-2</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>12.594959543681432</v>
+        <v>4.6018145392646597</v>
       </c>
       <c r="R17">
         <f t="shared" si="0"/>
@@ -11750,7 +11754,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>1.764367118624981</v>
+        <v>2.2312221545982647</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
@@ -11764,11 +11768,11 @@
       </c>
       <c r="E18">
         <f>G5*SIN(C18+H5)</f>
-        <v>-0.1383111543663833</v>
+        <v>-6.214620579765643E-2</v>
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>9.2354371417853898</v>
+        <v>4.1496825030057973</v>
       </c>
       <c r="R18">
         <f t="shared" si="0"/>
@@ -11776,7 +11780,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>1.9605864979711052</v>
+        <v>2.2576297973891402</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
@@ -11790,11 +11794,11 @@
       </c>
       <c r="E19">
         <f>G5*SIN(C19+H5)</f>
-        <v>-3.5168333050857307E-2</v>
+        <v>-3.1637276995598707E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>1.4513240568603978</v>
+        <v>1.3056047078167998</v>
       </c>
       <c r="R19">
         <f t="shared" si="0"/>
@@ -11802,7 +11806,7 @@
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>2.3628435011016564</v>
+        <v>2.3766146197171651</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.3">
@@ -11816,11 +11820,11 @@
       </c>
       <c r="E20">
         <f>G5*SIN(C20+H5)</f>
-        <v>8.140759616241991E-2</v>
+        <v>1.0956016307282565E-2</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>-1.4004821195703692E-15</v>
+        <v>-1.884800149295369E-16</v>
       </c>
       <c r="R20">
         <f t="shared" si="0"/>
@@ -11828,7 +11832,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>2.8174896250334376</v>
+        <v>2.5427284635984022</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
@@ -11842,11 +11846,11 @@
       </c>
       <c r="E21">
         <f>G5*SIN(C21+H5)</f>
-        <v>0.16688859058407823</v>
+        <v>4.9364483762080011E-2</v>
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>6.8871454890948787</v>
+        <v>2.0371697098863391</v>
       </c>
       <c r="R21">
         <f t="shared" si="0"/>
@@ -11854,7 +11858,7 @@
       </c>
       <c r="S21">
         <f t="shared" si="1"/>
-        <v>3.1508655032779052</v>
+        <v>2.6925214866721121</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
@@ -11871,11 +11875,11 @@
       </c>
       <c r="E22">
         <f>G5*SIN(C22+H6)</f>
-        <v>0.12658934851567041</v>
+        <v>4.6439874171398055E-2</v>
       </c>
       <c r="G22">
         <f t="shared" si="3"/>
-        <v>5.9158159018037928</v>
+        <v>2.1702437789773068</v>
       </c>
       <c r="R22">
         <f t="shared" si="0"/>
@@ -11883,7 +11887,7 @@
       </c>
       <c r="S22">
         <f t="shared" si="1"/>
-        <v>2.9936984592111147</v>
+        <v>2.6811155092684524</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
@@ -11901,11 +11905,11 @@
       </c>
       <c r="E23">
         <f>G5*SIN(C23+H5)</f>
-        <v>0.18525458995177932</v>
+        <v>6.9658563329342393E-2</v>
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
-        <v>12.709443839526381</v>
+        <v>4.7789455516692616</v>
       </c>
       <c r="R23">
         <f t="shared" si="0"/>
@@ -11913,7 +11917,7 @@
       </c>
       <c r="S23">
         <f t="shared" si="1"/>
-        <v>3.2224929008119392</v>
+        <v>2.7716683969844356</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
@@ -11927,11 +11931,11 @@
       </c>
       <c r="E24">
         <f>G5*SIN(C24+H5)</f>
-        <v>0.13831115436638336</v>
+        <v>6.2146205797656437E-2</v>
       </c>
       <c r="G24">
         <f t="shared" si="3"/>
-        <v>9.2354371417853915</v>
+        <v>4.1496825030057982</v>
       </c>
       <c r="R24">
         <f t="shared" si="0"/>
@@ -11939,7 +11943,7 @@
       </c>
       <c r="S24">
         <f t="shared" si="1"/>
-        <v>3.039413502028895</v>
+        <v>2.7423702026108603</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
@@ -11953,11 +11957,11 @@
       </c>
       <c r="E25">
         <f>G5*SIN(C25+H5)</f>
-        <v>1.6333379680583328E-2</v>
+        <v>2.5271134852668325E-2</v>
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>0.57805749674193163</v>
+        <v>0.89437515311831173</v>
       </c>
       <c r="R25">
         <f t="shared" si="0"/>
@@ -11965,7 +11969,7 @@
       </c>
       <c r="S25">
         <f t="shared" si="1"/>
-        <v>2.563700180754275</v>
+        <v>2.5985574259254065</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
@@ -11979,11 +11983,11 @@
       </c>
       <c r="E26">
         <f>G5*SIN(C26+H5)</f>
-        <v>-9.8160253481541046E-2</v>
+        <v>-1.7780224892352311E-2</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>0.68802707826324117</v>
+        <v>0.12462555616616219</v>
       </c>
       <c r="R26">
         <f t="shared" si="0"/>
@@ -11991,7 +11995,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
-        <v>2.11717501142199</v>
+        <v>2.4306571229198259</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
@@ -12005,11 +12009,11 @@
       </c>
       <c r="E27">
         <f>G5*SIN(C27+H5)</f>
-        <v>-0.17516000615802194</v>
+        <v>-5.4040143056111302E-2</v>
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
-        <v>8.1856361687603147</v>
+        <v>2.5254220941623751</v>
       </c>
       <c r="R27">
         <f t="shared" si="0"/>
@@ -12017,7 +12021,7 @@
       </c>
       <c r="S27">
         <f t="shared" si="1"/>
-        <v>1.8168759759837143</v>
+        <v>2.2892434420811658</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.3">
@@ -12031,11 +12035,11 @@
       </c>
       <c r="E28">
         <f>G5*SIN(C28+H5)</f>
-        <v>-0.18525458995177935</v>
+        <v>-6.9658563329342393E-2</v>
       </c>
       <c r="G28">
         <f t="shared" si="3"/>
-        <v>12.709443839526383</v>
+        <v>4.7789455516692616</v>
       </c>
       <c r="R28">
         <f t="shared" si="0"/>
@@ -12043,7 +12047,7 @@
       </c>
       <c r="S28">
         <f t="shared" si="1"/>
-        <v>1.7775070991880606</v>
+        <v>2.2283316030155644</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
@@ -12057,11 +12061,11 @@
       </c>
       <c r="E29">
         <f>G5*SIN(C29+H5)</f>
-        <v>-0.12458821695588179</v>
+        <v>-5.8669780018251731E-2</v>
       </c>
       <c r="G29">
         <f t="shared" si="3"/>
-        <v>8.0077016481302365</v>
+        <v>3.7709031048574868</v>
       </c>
       <c r="R29">
         <f t="shared" si="0"/>
@@ -12069,7 +12073,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>2.0141059538720611</v>
+        <v>2.2711878579288181</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.3">
@@ -12083,11 +12087,11 @@
       </c>
       <c r="E30">
         <f>G5*SIN(C30+H5)</f>
-        <v>-1.6333379680583349E-2</v>
+        <v>-2.5271134852668332E-2</v>
       </c>
       <c r="G30">
         <f t="shared" si="3"/>
-        <v>0.57805749674193307</v>
+        <v>0.89437515311831306</v>
       </c>
       <c r="R30">
         <f t="shared" si="0"/>
@@ -12095,7 +12099,7 @@
       </c>
       <c r="S30">
         <f t="shared" si="1"/>
-        <v>2.436299819245725</v>
+        <v>2.4014425740745935</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.3">
@@ -12109,11 +12113,11 @@
       </c>
       <c r="E31">
         <f>G5*SIN(C31+H5)</f>
-        <v>9.8160253481541018E-2</v>
+        <v>1.7780224892352304E-2</v>
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
-        <v>0.68802707826323706</v>
+        <v>0.12462555616616143</v>
       </c>
       <c r="R31">
         <f t="shared" si="0"/>
@@ -12121,7 +12125,7 @@
       </c>
       <c r="S31">
         <f t="shared" si="1"/>
-        <v>2.88282498857801</v>
+        <v>2.5693428770801741</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.3">
@@ -12135,11 +12139,11 @@
       </c>
       <c r="E32">
         <f>G5*SIN(C32+H5)</f>
-        <v>0.17516000615802191</v>
+        <v>5.4040143056111295E-2</v>
       </c>
       <c r="G32">
         <f t="shared" si="3"/>
-        <v>8.1856361687603076</v>
+        <v>2.5254220941623724</v>
       </c>
       <c r="R32">
         <f t="shared" si="0"/>
@@ -12147,7 +12151,7 @@
       </c>
       <c r="S32">
         <f t="shared" si="1"/>
-        <v>3.1831240240162852</v>
+        <v>2.7107565579188342</v>
       </c>
     </row>
     <row r="35" spans="3:24" x14ac:dyDescent="0.3">
@@ -12279,11 +12283,11 @@
       </c>
       <c r="S38">
         <f>(S37-P10)/P10*100</f>
-        <v>-2.6502193746460585</v>
+        <v>142.83666189108365</v>
       </c>
       <c r="T38">
         <f>(T37-P10)/P10*100</f>
-        <v>25.22758832010074</v>
+        <v>212.37717567495088</v>
       </c>
       <c r="U38" t="s">
         <v>337</v>
@@ -12294,11 +12298,11 @@
       </c>
       <c r="W38">
         <f>(W37-F5)/F5*100</f>
-        <v>-0.5562539171876536</v>
+        <v>171.07134235807499</v>
       </c>
       <c r="X38">
         <f>(X37-F5*SQRT(2))/(F5*SQRT(2))*100</f>
-        <v>-3.8864336945521356</v>
+        <v>161.99368450524062</v>
       </c>
     </row>
     <row r="39" spans="3:24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed to taking voltage then current then averaging instantaneous power, idk if I said that last commit but now it's accurate and specific to our pcb
</commit_message>
<xml_diff>
--- a/Firmware/EnergyMonitor/analysis.xlsx
+++ b/Firmware/EnergyMonitor/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y3J5bw\ownCloud\UoA\2024\Semester 2 2024\COMPSYS 209\ec209-project-2024_team_33\Firmware\EnergyMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE75C808-B303-432F-9A45-6FB5C072032C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF11513-7CB5-4F6E-B221-EF34938C94BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="26136" activeTab="1" xr2:uid="{5B712931-4F47-4E8C-8387-F250B08A1400}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="345">
   <si>
     <t>Phase</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Current</t>
   </si>
   <si>
-    <t>Assuming VRMS is 14V, Rs is 0.282ohms, Rload is 26.25 ohms</t>
-  </si>
-  <si>
     <t>XL</t>
   </si>
   <si>
@@ -1091,6 +1088,12 @@
   </si>
   <si>
     <t>Peak Current</t>
+  </si>
+  <si>
+    <t>Rsens</t>
+  </si>
+  <si>
+    <t>Proteus Value</t>
   </si>
 </sst>
 </file>
@@ -4760,40 +4763,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.5427284635984018</c:v>
+                  <c:v>2.5329260685009682</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6925214866721121</c:v>
+                  <c:v>2.672611432486768</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7687778454017353</c:v>
+                  <c:v>2.7463650961094301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7423702026108603</c:v>
+                  <c:v>2.726015666659924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6233853802828349</c:v>
+                  <c:v>2.6193359345362937</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4572715364015982</c:v>
+                  <c:v>2.4670739314990318</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3074785133278879</c:v>
+                  <c:v>2.327388567513232</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2312221545982647</c:v>
+                  <c:v>2.2536349038905699</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2576297973891402</c:v>
+                  <c:v>2.273984333340076</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3766146197171651</c:v>
+                  <c:v>2.3806640654637063</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5427284635984022</c:v>
+                  <c:v>2.5329260685009682</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.6925214866721121</c:v>
+                  <c:v>2.672611432486768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11424,37 +11427,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A733CF-01AB-433F-B8EB-89FAB0430329}">
-  <dimension ref="B3:AD137"/>
+  <dimension ref="B2:AD137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="2" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>343</v>
+      </c>
+    </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>17</v>
+      <c r="C3">
+        <v>15.4</v>
+      </c>
+      <c r="D3">
+        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>342</v>
+      </c>
+      <c r="P4" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.3">
@@ -11463,24 +11483,31 @@
         <v>12.566370614359172</v>
       </c>
       <c r="D5">
-        <f>105*0.75+0.282</f>
-        <v>79.031999999999996</v>
+        <f>105*0.9+0.282</f>
+        <v>94.781999999999996</v>
       </c>
       <c r="E5">
         <f>SQRT(SUMSQ(C5:D5))</f>
-        <v>80.024812992080328</v>
+        <v>95.611407240022501</v>
       </c>
       <c r="F5">
-        <f>14/E5</f>
-        <v>0.17494573840972941</v>
+        <f>C3/E5</f>
+        <v>0.16106864697995607</v>
       </c>
       <c r="G5">
         <f>F5*0.282*SQRT(2)</f>
-        <v>6.9769799334633037E-2</v>
+        <v>6.4235501139062942E-2</v>
       </c>
       <c r="H5">
         <f>ATAN(C5/D5)</f>
-        <v>0.1576835591301893</v>
+        <v>0.13181307897974545</v>
+      </c>
+      <c r="I5">
+        <f>F5*SQRT(2)</f>
+        <v>0.22778546503213815</v>
+      </c>
+      <c r="P5">
+        <v>2.41</v>
       </c>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.3">
@@ -11497,13 +11524,13 @@
         <v>3</v>
       </c>
       <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" t="s">
         <v>22</v>
       </c>
-      <c r="L9" t="s">
+      <c r="P9" t="s">
         <v>23</v>
-      </c>
-      <c r="P9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.3">
@@ -11517,7 +11544,7 @@
       </c>
       <c r="E10">
         <f>G5*SIN(C10+H5)</f>
-        <v>1.0956016307282553E-2</v>
+        <v>8.4425816669149757E-3</v>
       </c>
       <c r="G10">
         <f>D10*E10/0.282</f>
@@ -11525,7 +11552,7 @@
       </c>
       <c r="J10">
         <f>AVERAGE(G11:G32)</f>
-        <v>2.4074217603139245</v>
+        <v>2.2215378314538685</v>
       </c>
       <c r="L10">
         <f>SQRT(SUMSQ(D11:D32)/COUNT(D11:D32))</f>
@@ -11533,15 +11560,15 @@
       </c>
       <c r="M10">
         <f>SQRT(SUMSQ(E11:E32)/COUNT(E11:E32))/0.282</f>
-        <v>0.17518358748029594</v>
+        <v>0.16107859019027151</v>
       </c>
       <c r="N10">
         <f>L10*M10*COS(H5)</f>
-        <v>2.4061242845532713</v>
+        <v>2.2207532901056091</v>
       </c>
       <c r="P10">
-        <f>14*F5*COS(H5)</f>
-        <v>2.4188542919947187</v>
+        <f>C3*F5*COS(H5)</f>
+        <v>2.4589397610248924</v>
       </c>
       <c r="R10">
         <f>D10/23+2.5</f>
@@ -11549,7 +11576,7 @@
       </c>
       <c r="S10">
         <f>E10*3.9+2.5</f>
-        <v>2.5427284635984018</v>
+        <v>2.5329260685009682</v>
       </c>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.3">
@@ -11563,18 +11590,18 @@
       </c>
       <c r="E11">
         <f>G5*SIN(C11+H5)</f>
-        <v>4.936448376207999E-2</v>
+        <v>4.4259341663273853E-2</v>
       </c>
       <c r="G11">
         <f>D11*E11/0.282</f>
-        <v>2.0371697098863395</v>
+        <v>1.8264910993598305</v>
       </c>
       <c r="I11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J11">
         <f>(J10-P10)/P10*100</f>
-        <v>-0.47264242904711218</v>
+        <v>-9.6546460118272357</v>
       </c>
       <c r="L11">
         <f>(L10-14)/L10*100</f>
@@ -11582,15 +11609,15 @@
       </c>
       <c r="M11">
         <f>(M10-F5)/F5*100</f>
-        <v>0.13595590994590886</v>
+        <v>6.1732748749552431E-3</v>
       </c>
       <c r="N11">
         <f>(N10-P10)/P10*100</f>
-        <v>-0.52628252489526806</v>
+        <v>-9.6865516876268103</v>
       </c>
       <c r="P11">
-        <f>(2.38-P10)/P10*100</f>
-        <v>-1.6063097361138454</v>
+        <f>(P5-P10)/P10*100</f>
+        <v>-1.9902789731007504</v>
       </c>
       <c r="R11">
         <f t="shared" ref="R11:R32" si="0">D11/23+2.5</f>
@@ -11598,7 +11625,7 @@
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S32" si="1">E11*3.9+2.5</f>
-        <v>2.6925214866721121</v>
+        <v>2.672611432486768</v>
       </c>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.3">
@@ -11612,11 +11639,11 @@
       </c>
       <c r="E12">
         <f>G5*SIN(C12+H5)</f>
-        <v>6.8917396256855154E-2</v>
+        <v>6.3170537463956414E-2</v>
       </c>
       <c r="G12">
         <f t="shared" ref="G12:G32" si="3">D12*E12/0.282</f>
-        <v>4.6018145392646588</v>
+        <v>4.2180801008697699</v>
       </c>
       <c r="R12">
         <f t="shared" si="0"/>
@@ -11624,7 +11651,7 @@
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>2.7687778454017353</v>
+        <v>2.7463650961094301</v>
       </c>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.3">
@@ -11638,11 +11665,11 @@
       </c>
       <c r="E13">
         <f>G5*SIN(C13+H5)</f>
-        <v>6.2146205797656437E-2</v>
+        <v>5.7952735041006211E-2</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>4.1496825030057982</v>
+        <v>3.8696722915635058</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
@@ -11650,7 +11677,7 @@
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>2.7423702026108603</v>
+        <v>2.726015666659924</v>
       </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.3">
@@ -11664,11 +11691,11 @@
       </c>
       <c r="E14">
         <f>G5*SIN(C14+H5)</f>
-        <v>3.1637276995598727E-2</v>
+        <v>3.0598957573408671E-2</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>1.3056047078168003</v>
+        <v>1.2627554219564039</v>
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
@@ -11676,7 +11703,7 @@
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>2.6233853802828349</v>
+        <v>2.6193359345362937</v>
       </c>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.3">
@@ -11690,11 +11717,11 @@
       </c>
       <c r="E15">
         <f>G5*SIN(C15+H5)</f>
-        <v>-1.095601630728254E-2</v>
+        <v>-8.4425816669149775E-3</v>
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>-9.4240007464768242E-17</v>
+        <v>-7.2620278849267763E-17</v>
       </c>
       <c r="R15">
         <f t="shared" si="0"/>
@@ -11702,7 +11729,7 @@
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>2.4572715364015982</v>
+        <v>2.4670739314990318</v>
       </c>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.3">
@@ -11716,11 +11743,11 @@
       </c>
       <c r="E16">
         <f>G5*SIN(C16+H5)</f>
-        <v>-4.936448376207999E-2</v>
+        <v>-4.4259341663273846E-2</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>2.0371697098863391</v>
+        <v>1.8264910993598296</v>
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
@@ -11728,7 +11755,7 @@
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>2.3074785133278879</v>
+        <v>2.327388567513232</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
@@ -11742,11 +11769,11 @@
       </c>
       <c r="E17">
         <f>G5*SIN(C17+H5)</f>
-        <v>-6.8917396256855168E-2</v>
+        <v>-6.3170537463956414E-2</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>4.6018145392646597</v>
+        <v>4.2180801008697699</v>
       </c>
       <c r="R17">
         <f t="shared" si="0"/>
@@ -11754,7 +11781,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>2.2312221545982647</v>
+        <v>2.2536349038905699</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
@@ -11768,11 +11795,11 @@
       </c>
       <c r="E18">
         <f>G5*SIN(C18+H5)</f>
-        <v>-6.214620579765643E-2</v>
+        <v>-5.7952735041006218E-2</v>
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>4.1496825030057973</v>
+        <v>3.8696722915635067</v>
       </c>
       <c r="R18">
         <f t="shared" si="0"/>
@@ -11780,7 +11807,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>2.2576297973891402</v>
+        <v>2.273984333340076</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
@@ -11794,11 +11821,11 @@
       </c>
       <c r="E19">
         <f>G5*SIN(C19+H5)</f>
-        <v>-3.1637276995598707E-2</v>
+        <v>-3.0598957573408678E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>1.3056047078167998</v>
+        <v>1.2627554219564043</v>
       </c>
       <c r="R19">
         <f t="shared" si="0"/>
@@ -11806,7 +11833,7 @@
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>2.3766146197171651</v>
+        <v>2.3806640654637063</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.3">
@@ -11820,11 +11847,11 @@
       </c>
       <c r="E20">
         <f>G5*SIN(C20+H5)</f>
-        <v>1.0956016307282565E-2</v>
+        <v>8.4425816669149688E-3</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>-1.884800149295369E-16</v>
+        <v>-1.4524055769853538E-16</v>
       </c>
       <c r="R20">
         <f t="shared" si="0"/>
@@ -11832,7 +11859,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>2.5427284635984022</v>
+        <v>2.5329260685009682</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
@@ -11846,11 +11873,11 @@
       </c>
       <c r="E21">
         <f>G5*SIN(C21+H5)</f>
-        <v>4.9364483762080011E-2</v>
+        <v>4.4259341663273846E-2</v>
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>2.0371697098863391</v>
+        <v>1.8264910993598293</v>
       </c>
       <c r="R21">
         <f t="shared" si="0"/>
@@ -11858,12 +11885,12 @@
       </c>
       <c r="S21">
         <f t="shared" si="1"/>
-        <v>2.6925214866721121</v>
+        <v>2.672611432486768</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <f>C11+B23</f>
@@ -11875,11 +11902,11 @@
       </c>
       <c r="E22">
         <f>G5*SIN(C22+H6)</f>
-        <v>4.6439874171398055E-2</v>
+        <v>4.275615837630773E-2</v>
       </c>
       <c r="G22">
         <f t="shared" si="3"/>
-        <v>2.1702437789773068</v>
+        <v>1.9980951366638227</v>
       </c>
       <c r="R22">
         <f t="shared" si="0"/>
@@ -11887,7 +11914,7 @@
       </c>
       <c r="S22">
         <f t="shared" si="1"/>
-        <v>2.6811155092684524</v>
+        <v>2.6667490176676001</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
@@ -11905,11 +11932,11 @@
       </c>
       <c r="E23">
         <f>G5*SIN(C23+H5)</f>
-        <v>6.9658563329342393E-2</v>
+        <v>6.4017837101842542E-2</v>
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
-        <v>4.7789455516692616</v>
+        <v>4.3919619243204684</v>
       </c>
       <c r="R23">
         <f t="shared" si="0"/>
@@ -11917,7 +11944,7 @@
       </c>
       <c r="S23">
         <f t="shared" si="1"/>
-        <v>2.7716683969844356</v>
+        <v>2.7496695646971858</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
@@ -11931,11 +11958,11 @@
       </c>
       <c r="E24">
         <f>G5*SIN(C24+H5)</f>
-        <v>6.2146205797656437E-2</v>
+        <v>5.7952735041006211E-2</v>
       </c>
       <c r="G24">
         <f t="shared" si="3"/>
-        <v>4.1496825030057982</v>
+        <v>3.8696722915635058</v>
       </c>
       <c r="R24">
         <f t="shared" si="0"/>
@@ -11943,7 +11970,7 @@
       </c>
       <c r="S24">
         <f t="shared" si="1"/>
-        <v>2.7423702026108603</v>
+        <v>2.726015666659924</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
@@ -11957,11 +11984,11 @@
       </c>
       <c r="E25">
         <f>G5*SIN(C25+H5)</f>
-        <v>2.5271134852668325E-2</v>
+        <v>2.4807575755358302E-2</v>
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>0.89437515311831173</v>
+        <v>0.87796925203578624</v>
       </c>
       <c r="R25">
         <f t="shared" si="0"/>
@@ -11969,7 +11996,7 @@
       </c>
       <c r="S25">
         <f t="shared" si="1"/>
-        <v>2.5985574259254065</v>
+        <v>2.5967495454458973</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
@@ -11983,11 +12010,11 @@
       </c>
       <c r="E26">
         <f>G5*SIN(C26+H5)</f>
-        <v>-1.7780224892352311E-2</v>
+        <v>-1.4757623459834451E-2</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>0.12462555616616219</v>
+        <v>0.10343946955157717</v>
       </c>
       <c r="R26">
         <f t="shared" si="0"/>
@@ -11995,7 +12022,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
-        <v>2.4306571229198259</v>
+        <v>2.4424452685066456</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
@@ -12009,11 +12036,11 @@
       </c>
       <c r="E27">
         <f>G5*SIN(C27+H5)</f>
-        <v>-5.4040143056111302E-2</v>
+        <v>-4.8685912106543244E-2</v>
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
-        <v>2.5254220941623751</v>
+        <v>2.2752063772415805</v>
       </c>
       <c r="R27">
         <f t="shared" si="0"/>
@@ -12021,7 +12048,7 @@
       </c>
       <c r="S27">
         <f t="shared" si="1"/>
-        <v>2.2892434420811658</v>
+        <v>2.3101249427844812</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.3">
@@ -12035,11 +12062,11 @@
       </c>
       <c r="E28">
         <f>G5*SIN(C28+H5)</f>
-        <v>-6.9658563329342393E-2</v>
+        <v>-6.4017837101842542E-2</v>
       </c>
       <c r="G28">
         <f t="shared" si="3"/>
-        <v>4.7789455516692616</v>
+        <v>4.3919619243204684</v>
       </c>
       <c r="R28">
         <f t="shared" si="0"/>
@@ -12047,7 +12074,7 @@
       </c>
       <c r="S28">
         <f t="shared" si="1"/>
-        <v>2.2283316030155644</v>
+        <v>2.2503304353028142</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
@@ -12061,11 +12088,11 @@
       </c>
       <c r="E29">
         <f>G5*SIN(C29+H5)</f>
-        <v>-5.8669780018251731E-2</v>
+        <v>-5.4897124210492046E-2</v>
       </c>
       <c r="G29">
         <f t="shared" si="3"/>
-        <v>3.7709031048574868</v>
+        <v>3.528421890600097</v>
       </c>
       <c r="R29">
         <f t="shared" si="0"/>
@@ -12073,7 +12100,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>2.2711878579288181</v>
+        <v>2.2859012155790812</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.3">
@@ -12087,11 +12114,11 @@
       </c>
       <c r="E30">
         <f>G5*SIN(C30+H5)</f>
-        <v>-2.5271134852668332E-2</v>
+        <v>-2.4807575755358337E-2</v>
       </c>
       <c r="G30">
         <f t="shared" si="3"/>
-        <v>0.89437515311831306</v>
+        <v>0.87796925203578857</v>
       </c>
       <c r="R30">
         <f t="shared" si="0"/>
@@ -12099,7 +12126,7 @@
       </c>
       <c r="S30">
         <f t="shared" si="1"/>
-        <v>2.4014425740745935</v>
+        <v>2.4032504545541027</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.3">
@@ -12113,11 +12140,11 @@
       </c>
       <c r="E31">
         <f>G5*SIN(C31+H5)</f>
-        <v>1.7780224892352304E-2</v>
+        <v>1.4757623459834415E-2</v>
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
-        <v>0.12462555616616143</v>
+        <v>0.10343946955157633</v>
       </c>
       <c r="R31">
         <f t="shared" si="0"/>
@@ -12125,7 +12152,7 @@
       </c>
       <c r="S31">
         <f t="shared" si="1"/>
-        <v>2.5693428770801741</v>
+        <v>2.5575547314933544</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.3">
@@ -12139,11 +12166,11 @@
       </c>
       <c r="E32">
         <f>G5*SIN(C32+H5)</f>
-        <v>5.4040143056111295E-2</v>
+        <v>4.8685912106543237E-2</v>
       </c>
       <c r="G32">
         <f t="shared" si="3"/>
-        <v>2.5254220941623724</v>
+        <v>2.2752063772415787</v>
       </c>
       <c r="R32">
         <f t="shared" si="0"/>
@@ -12151,40 +12178,40 @@
       </c>
       <c r="S32">
         <f t="shared" si="1"/>
-        <v>2.7107565579188342</v>
+        <v>2.6898750572155188</v>
       </c>
     </row>
     <row r="35" spans="3:24" x14ac:dyDescent="0.3">
       <c r="K35" t="s">
+        <v>333</v>
+      </c>
+      <c r="N35" t="s">
         <v>334</v>
-      </c>
-      <c r="N35" t="s">
-        <v>335</v>
       </c>
       <c r="Q35" t="s">
         <v>3</v>
       </c>
       <c r="S35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="V35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="X35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="3:24" x14ac:dyDescent="0.3">
       <c r="V36" t="s">
+        <v>340</v>
+      </c>
+      <c r="W36" t="s">
         <v>341</v>
-      </c>
-      <c r="W36" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="37" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37">
         <v>800151</v>
@@ -12193,7 +12220,7 @@
         <v>601</v>
       </c>
       <c r="G37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H37" s="2">
         <v>80020</v>
@@ -12244,7 +12271,7 @@
     </row>
     <row r="38" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38">
         <v>800153</v>
@@ -12253,7 +12280,7 @@
         <v>670</v>
       </c>
       <c r="G38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H38" s="2">
         <v>8002000</v>
@@ -12283,31 +12310,31 @@
       </c>
       <c r="S38">
         <f>(S37-P10)/P10*100</f>
-        <v>142.83666189108365</v>
+        <v>138.87795511675887</v>
       </c>
       <c r="T38">
         <f>(T37-P10)/P10*100</f>
-        <v>212.37717567495088</v>
+        <v>207.28482416649743</v>
       </c>
       <c r="U38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="V38">
-        <f>(V37-14)/14*100</f>
-        <v>-6.8176224782437858E-2</v>
+        <f>(V37-14)/C3*100</f>
+        <v>-6.1978386165852592E-2</v>
       </c>
       <c r="W38">
         <f>(W37-F5)/F5*100</f>
-        <v>171.07134235807499</v>
+        <v>194.42586772614683</v>
       </c>
       <c r="X38">
         <f>(X37-F5*SQRT(2))/(F5*SQRT(2))*100</f>
-        <v>161.99368450524062</v>
+        <v>184.56611174090779</v>
       </c>
     </row>
     <row r="39" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39">
         <v>800155</v>
@@ -12316,7 +12343,7 @@
         <v>685</v>
       </c>
       <c r="G39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H39" s="2">
         <v>800200000</v>
@@ -12347,7 +12374,7 @@
     </row>
     <row r="40" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D40">
         <v>800157</v>
@@ -12356,7 +12383,7 @@
         <v>633</v>
       </c>
       <c r="G40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H40" s="2">
         <v>80020000000</v>
@@ -12387,7 +12414,7 @@
     </row>
     <row r="41" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D41">
         <v>800159</v>
@@ -12396,7 +12423,7 @@
         <v>536</v>
       </c>
       <c r="G41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H41" s="2">
         <v>8002000000000</v>
@@ -12427,19 +12454,19 @@
     </row>
     <row r="42" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E42">
         <v>429</v>
       </c>
       <c r="G42" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I42">
         <v>516</v>
@@ -12467,19 +12494,19 @@
     </row>
     <row r="43" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E43">
         <v>354</v>
       </c>
       <c r="G43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I43">
         <v>427</v>
@@ -12507,19 +12534,19 @@
     </row>
     <row r="44" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E44">
         <v>339</v>
       </c>
       <c r="G44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I44">
         <v>370</v>
@@ -12547,7 +12574,7 @@
     </row>
     <row r="45" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D45">
         <v>800161</v>
@@ -12556,10 +12583,10 @@
         <v>390</v>
       </c>
       <c r="G45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I45">
         <v>367</v>
@@ -12587,7 +12614,7 @@
     </row>
     <row r="46" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46">
         <v>800163</v>
@@ -12596,10 +12623,10 @@
         <v>488</v>
       </c>
       <c r="G46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I46">
         <v>419</v>
@@ -12627,7 +12654,7 @@
     </row>
     <row r="47" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D47">
         <v>800165</v>
@@ -12636,10 +12663,10 @@
         <v>595</v>
       </c>
       <c r="G47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I47">
         <v>508</v>
@@ -12667,7 +12694,7 @@
     </row>
     <row r="48" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D48">
         <v>800167</v>
@@ -12676,10 +12703,10 @@
         <v>671</v>
       </c>
       <c r="G48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I48">
         <v>597</v>
@@ -12707,7 +12734,7 @@
     </row>
     <row r="49" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D49">
         <v>800169</v>
@@ -12716,10 +12743,10 @@
         <v>685</v>
       </c>
       <c r="G49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I49">
         <v>654</v>
@@ -12747,19 +12774,19 @@
     </row>
     <row r="50" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E50">
         <v>634</v>
       </c>
       <c r="G50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I50">
         <v>657</v>
@@ -12787,19 +12814,19 @@
     </row>
     <row r="51" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E51">
         <v>536</v>
       </c>
       <c r="G51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H51" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I51">
         <v>605</v>
@@ -12827,19 +12854,19 @@
     </row>
     <row r="52" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E52">
         <v>429</v>
       </c>
       <c r="G52" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I52">
         <v>516</v>
@@ -12867,7 +12894,7 @@
     </row>
     <row r="53" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D53">
         <v>800171</v>
@@ -12876,7 +12903,7 @@
         <v>354</v>
       </c>
       <c r="G53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H53">
         <v>800301</v>
@@ -12907,7 +12934,7 @@
     </row>
     <row r="54" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D54">
         <v>800173</v>
@@ -12916,7 +12943,7 @@
         <v>339</v>
       </c>
       <c r="G54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H54">
         <v>800303</v>
@@ -12947,7 +12974,7 @@
     </row>
     <row r="55" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55">
         <v>800175</v>
@@ -12956,7 +12983,7 @@
         <v>390</v>
       </c>
       <c r="G55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H55">
         <v>800305</v>
@@ -12987,7 +13014,7 @@
     </row>
     <row r="56" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D56">
         <v>800177</v>
@@ -12996,7 +13023,7 @@
         <v>488</v>
       </c>
       <c r="G56" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H56">
         <v>800307</v>
@@ -13027,7 +13054,7 @@
     </row>
     <row r="57" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57">
         <v>800179</v>
@@ -13036,7 +13063,7 @@
         <v>583</v>
       </c>
       <c r="G57" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H57">
         <v>800309</v>
@@ -13067,19 +13094,19 @@
     </row>
     <row r="58" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E58">
         <v>664</v>
       </c>
       <c r="G58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H58" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I58">
         <v>597</v>
@@ -13107,19 +13134,19 @@
     </row>
     <row r="59" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E59">
         <v>687</v>
       </c>
       <c r="G59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H59" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I59">
         <v>654</v>
@@ -13148,19 +13175,19 @@
     </row>
     <row r="60" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E60">
         <v>643</v>
       </c>
       <c r="G60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I60">
         <v>657</v>
@@ -13193,7 +13220,7 @@
     </row>
     <row r="61" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61">
         <v>800181</v>
@@ -13202,7 +13229,7 @@
         <v>549</v>
       </c>
       <c r="G61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H61">
         <v>800311</v>
@@ -13234,7 +13261,7 @@
     </row>
     <row r="62" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D62">
         <v>800183</v>
@@ -13243,7 +13270,7 @@
         <v>441</v>
       </c>
       <c r="G62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H62">
         <v>800313</v>
@@ -13275,7 +13302,7 @@
     </row>
     <row r="63" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D63">
         <v>800185</v>
@@ -13284,7 +13311,7 @@
         <v>360</v>
       </c>
       <c r="G63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H63">
         <v>800315</v>
@@ -13316,7 +13343,7 @@
     </row>
     <row r="64" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D64">
         <v>800187</v>
@@ -13325,7 +13352,7 @@
         <v>337</v>
       </c>
       <c r="G64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H64">
         <v>800317</v>
@@ -13356,7 +13383,7 @@
     </row>
     <row r="65" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D65">
         <v>800189</v>
@@ -13365,7 +13392,7 @@
         <v>381</v>
       </c>
       <c r="G65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H65">
         <v>800319</v>
@@ -13396,19 +13423,19 @@
     </row>
     <row r="66" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E66">
         <v>475</v>
       </c>
       <c r="G66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H66" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I66">
         <v>420</v>
@@ -13436,19 +13463,19 @@
     </row>
     <row r="67" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E67">
         <v>583</v>
       </c>
       <c r="G67" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I67">
         <v>508</v>
@@ -13476,19 +13503,19 @@
     </row>
     <row r="68" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E68">
         <v>664</v>
       </c>
       <c r="G68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H68" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I68">
         <v>598</v>
@@ -13516,7 +13543,7 @@
     </row>
     <row r="69" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D69">
         <v>800191</v>
@@ -13525,7 +13552,7 @@
         <v>687</v>
       </c>
       <c r="G69" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H69">
         <v>800321</v>
@@ -13556,7 +13583,7 @@
     </row>
     <row r="70" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D70">
         <v>800193</v>
@@ -13565,7 +13592,7 @@
         <v>643</v>
       </c>
       <c r="G70" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H70">
         <v>800323</v>
@@ -13596,7 +13623,7 @@
     </row>
     <row r="71" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D71">
         <v>800195</v>
@@ -13605,7 +13632,7 @@
         <v>549</v>
       </c>
       <c r="G71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H71">
         <v>800325</v>
@@ -13636,7 +13663,7 @@
     </row>
     <row r="72" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D72">
         <v>800197</v>
@@ -13645,7 +13672,7 @@
         <v>441</v>
       </c>
       <c r="G72" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H72">
         <v>800327</v>
@@ -13676,7 +13703,7 @@
     </row>
     <row r="73" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D73">
         <v>800199</v>
@@ -13685,7 +13712,7 @@
         <v>360</v>
       </c>
       <c r="G73" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H73">
         <v>800329</v>
@@ -13716,19 +13743,19 @@
     </row>
     <row r="74" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E74">
         <v>337</v>
       </c>
       <c r="G74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H74" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I74">
         <v>370</v>
@@ -13756,19 +13783,19 @@
     </row>
     <row r="75" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E75">
         <v>381</v>
       </c>
       <c r="G75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H75" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I75">
         <v>367</v>
@@ -13796,19 +13823,19 @@
     </row>
     <row r="76" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E76">
         <v>475</v>
       </c>
       <c r="G76" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I76">
         <v>420</v>
@@ -13836,16 +13863,16 @@
     </row>
     <row r="77" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E77">
         <v>583</v>
       </c>
       <c r="G77" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H77">
         <v>800331</v>
@@ -13876,16 +13903,16 @@
     </row>
     <row r="78" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E78">
         <v>664</v>
       </c>
       <c r="G78" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H78">
         <v>800333</v>
@@ -13916,16 +13943,16 @@
     </row>
     <row r="79" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E79">
         <v>687</v>
       </c>
       <c r="G79" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H79">
         <v>800335</v>
@@ -13956,16 +13983,16 @@
     </row>
     <row r="80" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E80">
         <v>643</v>
       </c>
       <c r="G80" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H80">
         <v>800337</v>
@@ -13996,16 +14023,16 @@
     </row>
     <row r="81" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E81">
         <v>549</v>
       </c>
       <c r="G81" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H81">
         <v>800339</v>
@@ -14036,19 +14063,19 @@
     </row>
     <row r="82" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E82">
         <v>441</v>
       </c>
       <c r="G82" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I82">
         <v>516</v>
@@ -14076,19 +14103,19 @@
     </row>
     <row r="83" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E83">
         <v>360</v>
       </c>
       <c r="G83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H83" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I83">
         <v>426</v>
@@ -14116,19 +14143,19 @@
     </row>
     <row r="84" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E84">
         <v>337</v>
       </c>
       <c r="G84" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H84" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I84">
         <v>370</v>
@@ -14156,16 +14183,16 @@
     </row>
     <row r="85" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D85" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E85">
         <v>381</v>
       </c>
       <c r="G85" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H85">
         <v>800341</v>
@@ -14196,16 +14223,16 @@
     </row>
     <row r="86" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E86">
         <v>475</v>
       </c>
       <c r="G86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H86">
         <v>800343</v>
@@ -14236,16 +14263,16 @@
     </row>
     <row r="87" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E87">
         <v>583</v>
       </c>
       <c r="G87" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H87">
         <v>800345</v>
@@ -14276,16 +14303,16 @@
     </row>
     <row r="88" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E88">
         <v>664</v>
       </c>
       <c r="G88" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H88">
         <v>800347</v>
@@ -14316,16 +14343,16 @@
     </row>
     <row r="89" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E89">
         <v>687</v>
       </c>
       <c r="G89" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H89">
         <v>800349</v>
@@ -14356,19 +14383,19 @@
     </row>
     <row r="90" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D90" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E90">
         <v>643</v>
       </c>
       <c r="G90" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H90" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I90">
         <v>657</v>
@@ -14396,19 +14423,19 @@
     </row>
     <row r="91" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E91">
         <v>549</v>
       </c>
       <c r="G91" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H91" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I91">
         <v>604</v>
@@ -14436,19 +14463,19 @@
     </row>
     <row r="92" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E92">
         <v>441</v>
       </c>
       <c r="G92" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H92" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I92">
         <v>516</v>
@@ -14476,16 +14503,16 @@
     </row>
     <row r="93" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E93">
         <v>360</v>
       </c>
       <c r="G93" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H93">
         <v>800351</v>
@@ -14516,16 +14543,16 @@
     </row>
     <row r="94" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D94" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E94">
         <v>337</v>
       </c>
       <c r="G94" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H94">
         <v>800353</v>
@@ -14556,16 +14583,16 @@
     </row>
     <row r="95" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D95" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E95">
         <v>381</v>
       </c>
       <c r="G95" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H95">
         <v>800355</v>
@@ -14596,16 +14623,16 @@
     </row>
     <row r="96" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D96" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E96">
         <v>475</v>
       </c>
       <c r="G96" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H96">
         <v>800357</v>
@@ -14636,16 +14663,16 @@
     </row>
     <row r="97" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D97" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E97">
         <v>583</v>
       </c>
       <c r="G97" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H97">
         <v>800359</v>
@@ -14676,19 +14703,19 @@
     </row>
     <row r="98" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D98" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E98">
         <v>664</v>
       </c>
       <c r="G98" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H98" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I98">
         <v>597</v>
@@ -14716,19 +14743,19 @@
     </row>
     <row r="99" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C99" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D99" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E99">
         <v>687</v>
       </c>
       <c r="G99" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I99">
         <v>654</v>
@@ -14756,19 +14783,19 @@
     </row>
     <row r="100" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D100" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E100">
         <v>643</v>
       </c>
       <c r="G100" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H100" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I100">
         <v>657</v>
@@ -14796,16 +14823,16 @@
     </row>
     <row r="101" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C101" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D101" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E101">
         <v>549</v>
       </c>
       <c r="G101" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H101">
         <v>800361</v>
@@ -14836,16 +14863,16 @@
     </row>
     <row r="102" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D102" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E102">
         <v>441</v>
       </c>
       <c r="G102" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H102">
         <v>800363</v>
@@ -14876,16 +14903,16 @@
     </row>
     <row r="103" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C103" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E103">
         <v>360</v>
       </c>
       <c r="G103" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H103">
         <v>800365</v>
@@ -14916,16 +14943,16 @@
     </row>
     <row r="104" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C104" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E104">
         <v>337</v>
       </c>
       <c r="G104" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H104">
         <v>800367</v>
@@ -14956,16 +14983,16 @@
     </row>
     <row r="105" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C105" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E105">
         <v>381</v>
       </c>
       <c r="G105" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H105">
         <v>800369</v>
@@ -14996,19 +15023,19 @@
     </row>
     <row r="106" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C106" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E106">
         <v>475</v>
       </c>
       <c r="G106" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H106" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I106">
         <v>420</v>
@@ -15036,19 +15063,19 @@
     </row>
     <row r="107" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C107" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E107">
         <v>583</v>
       </c>
       <c r="G107" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H107" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I107">
         <v>508</v>
@@ -15076,19 +15103,19 @@
     </row>
     <row r="108" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C108" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E108">
         <v>664</v>
       </c>
       <c r="G108" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H108" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I108">
         <v>597</v>
@@ -15116,7 +15143,7 @@
     </row>
     <row r="109" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C109" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D109" s="2">
         <v>80010</v>
@@ -15125,7 +15152,7 @@
         <v>687</v>
       </c>
       <c r="G109" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H109">
         <v>800371</v>
@@ -15156,7 +15183,7 @@
     </row>
     <row r="110" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C110" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D110" s="2">
         <v>8001000</v>
@@ -15165,7 +15192,7 @@
         <v>643</v>
       </c>
       <c r="G110" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H110">
         <v>800373</v>
@@ -15196,7 +15223,7 @@
     </row>
     <row r="111" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D111" s="2">
         <v>800100000</v>
@@ -15205,7 +15232,7 @@
         <v>549</v>
       </c>
       <c r="G111" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H111">
         <v>800375</v>
@@ -15236,7 +15263,7 @@
     </row>
     <row r="112" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D112" s="2">
         <v>80010000000</v>
@@ -15245,7 +15272,7 @@
         <v>441</v>
       </c>
       <c r="G112" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H112">
         <v>800377</v>
@@ -15276,7 +15303,7 @@
     </row>
     <row r="113" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C113" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D113" s="2">
         <v>8001000000000</v>
@@ -15285,7 +15312,7 @@
         <v>360</v>
       </c>
       <c r="G113" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H113">
         <v>800379</v>
@@ -15316,19 +15343,19 @@
     </row>
     <row r="114" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C114" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D114" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E114">
         <v>337</v>
       </c>
       <c r="G114" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H114" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I114">
         <v>370</v>
@@ -15356,19 +15383,19 @@
     </row>
     <row r="115" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C115" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D115" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E115">
         <v>381</v>
       </c>
       <c r="G115" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H115" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I115">
         <v>367</v>
@@ -15396,19 +15423,19 @@
     </row>
     <row r="116" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C116" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D116" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E116">
         <v>475</v>
       </c>
       <c r="G116" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H116" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I116">
         <v>420</v>
@@ -15436,16 +15463,16 @@
     </row>
     <row r="117" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C117" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D117" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E117">
         <v>583</v>
       </c>
       <c r="G117" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H117">
         <v>800381</v>
@@ -15476,16 +15503,16 @@
     </row>
     <row r="118" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C118" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D118" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E118">
         <v>664</v>
       </c>
       <c r="G118" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H118">
         <v>800383</v>
@@ -15516,16 +15543,16 @@
     </row>
     <row r="119" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C119" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D119" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E119">
         <v>687</v>
       </c>
       <c r="G119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H119">
         <v>800385</v>
@@ -15556,16 +15583,16 @@
     </row>
     <row r="120" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C120" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D120" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E120">
         <v>643</v>
       </c>
       <c r="G120" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H120">
         <v>800387</v>
@@ -15596,16 +15623,16 @@
     </row>
     <row r="121" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C121" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D121" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E121">
         <v>549</v>
       </c>
       <c r="G121" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H121">
         <v>800389</v>
@@ -15636,19 +15663,19 @@
     </row>
     <row r="122" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C122" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D122" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E122">
         <v>441</v>
       </c>
       <c r="G122" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H122" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I122">
         <v>516</v>
@@ -15676,19 +15703,19 @@
     </row>
     <row r="123" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D123" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E123">
         <v>360</v>
       </c>
       <c r="G123" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H123" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I123">
         <v>426</v>
@@ -15716,19 +15743,19 @@
     </row>
     <row r="124" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C124" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D124" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E124">
         <v>337</v>
       </c>
       <c r="G124" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H124" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I124">
         <v>370</v>
@@ -15756,7 +15783,7 @@
     </row>
     <row r="125" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C125" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D125">
         <v>800201</v>
@@ -15765,7 +15792,7 @@
         <v>381</v>
       </c>
       <c r="G125" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H125">
         <v>800391</v>
@@ -15796,7 +15823,7 @@
     </row>
     <row r="126" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C126" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D126">
         <v>800203</v>
@@ -15805,7 +15832,7 @@
         <v>475</v>
       </c>
       <c r="G126" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H126">
         <v>800393</v>
@@ -15836,7 +15863,7 @@
     </row>
     <row r="127" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C127" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D127">
         <v>800205</v>
@@ -15845,7 +15872,7 @@
         <v>583</v>
       </c>
       <c r="G127" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H127">
         <v>800395</v>
@@ -15876,7 +15903,7 @@
     </row>
     <row r="128" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C128" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D128">
         <v>800207</v>
@@ -15885,7 +15912,7 @@
         <v>664</v>
       </c>
       <c r="G128" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H128">
         <v>800397</v>
@@ -15916,7 +15943,7 @@
     </row>
     <row r="129" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C129" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D129">
         <v>800209</v>
@@ -15925,7 +15952,7 @@
         <v>687</v>
       </c>
       <c r="G129" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H129">
         <v>800399</v>
@@ -15956,19 +15983,19 @@
     </row>
     <row r="130" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D130" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E130">
         <v>643</v>
       </c>
       <c r="G130" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H130" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I130">
         <v>657</v>
@@ -15996,19 +16023,19 @@
     </row>
     <row r="131" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C131" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D131" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E131">
         <v>549</v>
       </c>
       <c r="G131" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H131" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I131">
         <v>604</v>
@@ -16036,19 +16063,19 @@
     </row>
     <row r="132" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C132" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D132" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E132">
         <v>441</v>
       </c>
       <c r="G132" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H132" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I132">
         <v>516</v>
@@ -16076,7 +16103,7 @@
     </row>
     <row r="133" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C133" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D133">
         <v>800211</v>
@@ -16085,10 +16112,10 @@
         <v>360</v>
       </c>
       <c r="G133" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H133" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I133">
         <v>426</v>
@@ -16116,7 +16143,7 @@
     </row>
     <row r="134" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C134" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D134">
         <v>800213</v>
@@ -16125,10 +16152,10 @@
         <v>337</v>
       </c>
       <c r="G134" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H134" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I134">
         <v>370</v>
@@ -16156,7 +16183,7 @@
     </row>
     <row r="135" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C135" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D135">
         <v>800215</v>
@@ -16165,10 +16192,10 @@
         <v>381</v>
       </c>
       <c r="G135" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H135" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I135">
         <v>367</v>
@@ -16196,7 +16223,7 @@
     </row>
     <row r="136" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C136" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D136">
         <v>800217</v>
@@ -16205,10 +16232,10 @@
         <v>475</v>
       </c>
       <c r="G136" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H136" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I136">
         <v>420</v>
@@ -16236,7 +16263,7 @@
     </row>
     <row r="137" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C137" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D137">
         <v>800219</v>
@@ -16245,10 +16272,10 @@
         <v>583</v>
       </c>
       <c r="G137" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H137" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I137">
         <v>508</v>

</xml_diff>

<commit_message>
Fixed calculations and is very accurate in proteus now
</commit_message>
<xml_diff>
--- a/Firmware/EnergyMonitor/analysis.xlsx
+++ b/Firmware/EnergyMonitor/analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y3J5bw\ownCloud\UoA\2024\Semester 2 2024\COMPSYS 209\ec209-project-2024_team_33\Firmware\EnergyMonitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse Li\ownCloud\UoA\2024\Semester 2 2024\COMPSYS 209\ec209-project-2024_team_33\Firmware\EnergyMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF11513-7CB5-4F6E-B221-EF34938C94BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF8DE13-76DC-4421-8DBE-2AFFB298105B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="26136" activeTab="1" xr2:uid="{5B712931-4F47-4E8C-8387-F250B08A1400}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5B712931-4F47-4E8C-8387-F250B08A1400}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4763,40 +4763,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.5329260685009682</c:v>
+                  <c:v>2.8308778591034098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.672611432486768</c:v>
+                  <c:v>3.1680115606657169</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7463650961094301</c:v>
+                  <c:v>3.2499875509315821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.726015666659924</c:v>
+                  <c:v>3.0454937878808761</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6193359345362937</c:v>
+                  <c:v>2.6326399385116011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4670739314990318</c:v>
+                  <c:v>2.1691221408965902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.327388567513232</c:v>
+                  <c:v>1.8319884393342831</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2536349038905699</c:v>
+                  <c:v>1.7500124490684177</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.273984333340076</c:v>
+                  <c:v>1.9545062121191239</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3806640654637063</c:v>
+                  <c:v>2.3673600614883994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5329260685009682</c:v>
+                  <c:v>2.8308778591034098</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.672611432486768</c:v>
+                  <c:v>3.1680115606657169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8813,21 +8813,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88EF616-250D-46CA-B716-E8A9B416F08C}">
   <dimension ref="E5:AD90"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Y50" sqref="Y50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="26" max="27" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>3816</v>
       </c>
@@ -8835,12 +8835,12 @@
         <v>43828</v>
       </c>
     </row>
-    <row r="9" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>397</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>1.025390625</v>
       </c>
     </row>
-    <row r="11" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>645</v>
       </c>
@@ -8888,7 +8888,7 @@
         <v>1.8359375</v>
       </c>
     </row>
-    <row r="12" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>846</v>
       </c>
@@ -8924,7 +8924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>920</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>23.522786436404747</v>
       </c>
     </row>
-    <row r="14" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>838</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>-3.9686265039121884</v>
       </c>
     </row>
-    <row r="15" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>632</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>-1.025390625</v>
       </c>
     </row>
-    <row r="16" spans="5:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>379</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>-1.8359375</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>177</v>
       </c>
@@ -9079,7 +9079,7 @@
         <v>-1.943359375</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>105</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>-1.30859375</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>186</v>
       </c>
@@ -9127,7 +9127,7 @@
         <v>-0.17578125</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>382</v>
       </c>
@@ -9151,7 +9151,7 @@
         <v>0.966796875</v>
       </c>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>631</v>
       </c>
@@ -9175,7 +9175,7 @@
         <v>1.806640625</v>
       </c>
     </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>837</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>1.962890625</v>
       </c>
     </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>919</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>1.3671875</v>
       </c>
     </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>847</v>
       </c>
@@ -9247,7 +9247,7 @@
         <v>0.25390625</v>
       </c>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>647</v>
       </c>
@@ -9271,7 +9271,7 @@
         <v>-0.966796875</v>
       </c>
     </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>394</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>-1.806640625</v>
       </c>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>186</v>
       </c>
@@ -9319,7 +9319,7 @@
         <v>-1.953125</v>
       </c>
     </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>104</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>-1.357421875</v>
       </c>
     </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>176</v>
       </c>
@@ -9367,7 +9367,7 @@
         <v>-0.25390625</v>
       </c>
     </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>368</v>
       </c>
@@ -9391,7 +9391,7 @@
         <v>0.8984375</v>
       </c>
     </row>
-    <row r="31" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>616</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>1.77734375</v>
       </c>
     </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>828</v>
       </c>
@@ -9439,7 +9439,7 @@
         <v>1.97265625</v>
       </c>
     </row>
-    <row r="33" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>919</v>
       </c>
@@ -9463,7 +9463,7 @@
         <v>1.416015625</v>
       </c>
     </row>
-    <row r="34" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>855</v>
       </c>
@@ -9487,7 +9487,7 @@
         <v>0.322265625</v>
       </c>
     </row>
-    <row r="35" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>660</v>
       </c>
@@ -9511,7 +9511,7 @@
         <v>-0.8984375</v>
       </c>
     </row>
-    <row r="36" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>408</v>
       </c>
@@ -9538,7 +9538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>195</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>-1.962890625</v>
       </c>
     </row>
-    <row r="38" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>103</v>
       </c>
@@ -9589,7 +9589,7 @@
         <v>43978</v>
       </c>
     </row>
-    <row r="39" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>168</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>364</v>
       </c>
@@ -9696,7 +9696,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>616</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>6.0337732462844205</v>
       </c>
     </row>
-    <row r="42" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>827</v>
       </c>
@@ -9831,7 +9831,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>919</v>
       </c>
@@ -9880,7 +9880,7 @@
         <v>0.16902043269230771</v>
       </c>
     </row>
-    <row r="44" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>855</v>
       </c>
@@ -9929,7 +9929,7 @@
         <v>8.7640224358974367E-2</v>
       </c>
     </row>
-    <row r="45" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>660</v>
       </c>
@@ -9978,7 +9978,7 @@
         <v>-2.7544070512820512E-2</v>
       </c>
     </row>
-    <row r="46" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>408</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>-0.13271233974358976</v>
       </c>
     </row>
-    <row r="47" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>195</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>-0.18654847756410256</v>
       </c>
     </row>
-    <row r="48" spans="5:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:30" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>103</v>
       </c>
@@ -10125,7 +10125,7 @@
         <v>-0.16902043269230771</v>
       </c>
     </row>
-    <row r="49" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E49">
         <v>168</v>
       </c>
@@ -10174,7 +10174,7 @@
         <v>-8.7640224358974367E-2</v>
       </c>
     </row>
-    <row r="50" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E50">
         <v>364</v>
       </c>
@@ -10223,7 +10223,7 @@
         <v>4.8828125E-2</v>
       </c>
     </row>
-    <row r="51" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E51">
         <v>616</v>
       </c>
@@ -10272,7 +10272,7 @@
         <v>0.146484375</v>
       </c>
     </row>
-    <row r="52" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E52">
         <v>829</v>
       </c>
@@ -10321,7 +10321,7 @@
         <v>0.18905248397435898</v>
       </c>
     </row>
-    <row r="53" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E53">
         <v>920</v>
       </c>
@@ -10370,7 +10370,7 @@
         <v>0.16025641025641027</v>
       </c>
     </row>
-    <row r="54" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E54">
         <v>856</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>6.886017628205128E-2</v>
       </c>
     </row>
-    <row r="55" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E55">
         <v>660</v>
       </c>
@@ -10468,7 +10468,7 @@
         <v>-4.8828125E-2</v>
       </c>
     </row>
-    <row r="56" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E56">
         <v>408</v>
       </c>
@@ -10517,7 +10517,7 @@
         <v>-0.146484375</v>
       </c>
     </row>
-    <row r="57" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E57">
         <v>195</v>
       </c>
@@ -10550,7 +10550,7 @@
         <v>-0.18905248397435898</v>
       </c>
     </row>
-    <row r="58" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E58">
         <v>103</v>
       </c>
@@ -10583,7 +10583,7 @@
         <v>-0.15900440705128205</v>
       </c>
     </row>
-    <row r="59" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E59">
         <v>168</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>-4.3820112179487183E-2</v>
       </c>
     </row>
-    <row r="60" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>5</v>
       </c>
@@ -10646,7 +10646,7 @@
         <v>7.0112179487179488E-2</v>
       </c>
     </row>
-    <row r="61" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>6</v>
       </c>
@@ -10676,7 +10676,7 @@
         <v>0.16025641025641027</v>
       </c>
     </row>
-    <row r="62" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:24" x14ac:dyDescent="0.25">
       <c r="P62">
         <v>23</v>
       </c>
@@ -10703,7 +10703,7 @@
         <v>0.18905248397435898</v>
       </c>
     </row>
-    <row r="63" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:24" x14ac:dyDescent="0.25">
       <c r="P63">
         <v>24</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>0.146484375</v>
       </c>
     </row>
-    <row r="64" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:24" x14ac:dyDescent="0.25">
       <c r="P64">
         <v>25</v>
       </c>
@@ -10757,7 +10757,7 @@
         <v>4.7576121794871799E-2</v>
       </c>
     </row>
-    <row r="65" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="65" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P65">
         <v>26</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>-7.0112179487179488E-2</v>
       </c>
     </row>
-    <row r="66" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="66" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P66">
         <v>27</v>
       </c>
@@ -10815,7 +10815,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="67" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P67">
         <v>28</v>
       </c>
@@ -10842,7 +10842,7 @@
         <v>-0.18905248397435898</v>
       </c>
     </row>
-    <row r="68" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="68" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P68">
         <v>29</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>-0.146484375</v>
       </c>
     </row>
-    <row r="69" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="69" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P69">
         <v>30</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>-2.5040064102564104E-2</v>
       </c>
     </row>
-    <row r="70" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="70" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P70">
         <v>31</v>
       </c>
@@ -10923,7 +10923,7 @@
         <v>8.6388221153846159E-2</v>
       </c>
     </row>
-    <row r="71" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="71" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P71">
         <v>32</v>
       </c>
@@ -10950,7 +10950,7 @@
         <v>0.16902043269230771</v>
       </c>
     </row>
-    <row r="72" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="72" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P72">
         <v>33</v>
       </c>
@@ -10977,7 +10977,7 @@
         <v>0.18780048076923078</v>
       </c>
     </row>
-    <row r="73" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="73" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P73">
         <v>34</v>
       </c>
@@ -11004,7 +11004,7 @@
         <v>0.13396434294871795</v>
       </c>
     </row>
-    <row r="74" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="74" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P74">
         <v>35</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v>2.879607371794872E-2</v>
       </c>
     </row>
-    <row r="75" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="75" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P75">
         <v>36</v>
       </c>
@@ -11058,7 +11058,7 @@
         <v>-8.7640224358974367E-2</v>
       </c>
     </row>
-    <row r="76" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="76" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P76">
         <v>37</v>
       </c>
@@ -11085,7 +11085,7 @@
         <v>-0.1702724358974359</v>
       </c>
     </row>
-    <row r="77" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="77" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P77">
         <v>38</v>
       </c>
@@ -11112,7 +11112,7 @@
         <v>-0.18654847756410256</v>
       </c>
     </row>
-    <row r="78" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="78" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P78">
         <v>39</v>
       </c>
@@ -11139,7 +11139,7 @@
         <v>-0.13271233974358976</v>
       </c>
     </row>
-    <row r="79" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="79" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P79">
         <v>40</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>1.2520032051282052E-2</v>
       </c>
     </row>
-    <row r="80" spans="16:27" x14ac:dyDescent="0.3">
+    <row r="80" spans="16:27" x14ac:dyDescent="0.25">
       <c r="P80">
         <v>41</v>
       </c>
@@ -11193,7 +11193,7 @@
         <v>0.1201923076923077</v>
       </c>
     </row>
-    <row r="81" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="81" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P81">
         <v>42</v>
       </c>
@@ -11220,7 +11220,7 @@
         <v>0.18279246794871795</v>
       </c>
     </row>
-    <row r="82" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="82" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P82">
         <v>43</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>0.17653245192307693</v>
       </c>
     </row>
-    <row r="83" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="83" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P83">
         <v>44</v>
       </c>
@@ -11274,7 +11274,7 @@
         <v>0.10141225961538462</v>
       </c>
     </row>
-    <row r="84" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="84" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P84">
         <v>45</v>
       </c>
@@ -11301,7 +11301,7 @@
         <v>-1.2520032051282052E-2</v>
       </c>
     </row>
-    <row r="85" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="85" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P85">
         <v>46</v>
       </c>
@@ -11328,7 +11328,7 @@
         <v>-0.1214443108974359</v>
       </c>
     </row>
-    <row r="86" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="86" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P86">
         <v>47</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>-0.18279246794871795</v>
       </c>
     </row>
-    <row r="87" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="87" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P87">
         <v>48</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>-0.17653245192307693</v>
       </c>
     </row>
-    <row r="88" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="88" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P88">
         <v>49</v>
       </c>
@@ -11409,12 +11409,12 @@
         <v>-0.10141225961538462</v>
       </c>
     </row>
-    <row r="89" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="89" spans="16:24" x14ac:dyDescent="0.25">
       <c r="Q89" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="16:24" x14ac:dyDescent="0.3">
+    <row r="90" spans="16:24" x14ac:dyDescent="0.25">
       <c r="Q90" t="s">
         <v>13</v>
       </c>
@@ -11429,13 +11429,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A733CF-01AB-433F-B8EB-89FAB0430329}">
   <dimension ref="B2:AD137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="L38" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -11443,15 +11443,15 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3">
-        <v>15.4</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>0.28199999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
+        <v>0.3064600326264274</v>
+      </c>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>17</v>
       </c>
@@ -11473,44 +11473,48 @@
       <c r="I4" t="s">
         <v>342</v>
       </c>
+      <c r="K4">
+        <f>F5/0.1305</f>
+        <v>3.7305088196958516</v>
+      </c>
       <c r="P4" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C5">
         <f>2*PI()*500*0.004</f>
         <v>12.566370614359172</v>
       </c>
       <c r="D5">
-        <f>105*0.9+0.282</f>
-        <v>94.781999999999996</v>
+        <f>25.56+D3</f>
+        <v>25.866460032626428</v>
       </c>
       <c r="E5">
         <f>SQRT(SUMSQ(C5:D5))</f>
-        <v>95.611407240022501</v>
+        <v>28.757389051109804</v>
       </c>
       <c r="F5">
         <f>C3/E5</f>
-        <v>0.16106864697995607</v>
+        <v>0.48683140097030864</v>
       </c>
       <c r="G5">
         <f>F5*0.282*SQRT(2)</f>
-        <v>6.4235501139062942E-2</v>
+        <v>0.19415236669524796</v>
       </c>
       <c r="H5">
         <f>ATAN(C5/D5)</f>
-        <v>0.13181307897974545</v>
+        <v>0.452237110492829</v>
       </c>
       <c r="I5">
         <f>F5*SQRT(2)</f>
-        <v>0.22778546503213815</v>
+        <v>0.68848356984130488</v>
       </c>
       <c r="P5">
         <v>2.41</v>
       </c>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>14</v>
       </c>
@@ -11533,7 +11537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C10">
         <f>2*PI()/10*0</f>
         <v>0</v>
@@ -11544,7 +11548,7 @@
       </c>
       <c r="E10">
         <f>G5*SIN(C10+H5)</f>
-        <v>8.4425816669149757E-3</v>
+        <v>8.4840476693182065E-2</v>
       </c>
       <c r="G10">
         <f>D10*E10/0.282</f>
@@ -11552,7 +11556,7 @@
       </c>
       <c r="J10">
         <f>AVERAGE(G11:G32)</f>
-        <v>2.2215378314538685</v>
+        <v>6.2261769064245671</v>
       </c>
       <c r="L10">
         <f>SQRT(SUMSQ(D11:D32)/COUNT(D11:D32))</f>
@@ -11560,15 +11564,15 @@
       </c>
       <c r="M10">
         <f>SQRT(SUMSQ(E11:E32)/COUNT(E11:E32))/0.282</f>
-        <v>0.16107859019027151</v>
+        <v>0.49388357418898887</v>
       </c>
       <c r="N10">
         <f>L10*M10*COS(H5)</f>
-        <v>2.2207532901056091</v>
+        <v>6.1781502056995325</v>
       </c>
       <c r="P10">
         <f>C3*F5*COS(H5)</f>
-        <v>2.4589397610248924</v>
+        <v>6.1304755222470604</v>
       </c>
       <c r="R10">
         <f>D10/23+2.5</f>
@@ -11576,10 +11580,10 @@
       </c>
       <c r="S10">
         <f>E10*3.9+2.5</f>
-        <v>2.5329260685009682</v>
-      </c>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
+        <v>2.8308778591034098</v>
+      </c>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11">
         <f>2*PI()/10*1</f>
         <v>0.62831853071795862</v>
@@ -11590,18 +11594,18 @@
       </c>
       <c r="E11">
         <f>G5*SIN(C11+H5)</f>
-        <v>4.4259341663273853E-2</v>
+        <v>0.17128501555531203</v>
       </c>
       <c r="G11">
         <f>D11*E11/0.282</f>
-        <v>1.8264910993598305</v>
+        <v>7.0685768158429045</v>
       </c>
       <c r="I11" t="s">
         <v>24</v>
       </c>
       <c r="J11">
         <f>(J10-P10)/P10*100</f>
-        <v>-9.6546460118272357</v>
+        <v>1.5610760344807382</v>
       </c>
       <c r="L11">
         <f>(L10-14)/L10*100</f>
@@ -11609,15 +11613,15 @@
       </c>
       <c r="M11">
         <f>(M10-F5)/F5*100</f>
-        <v>6.1732748749552431E-3</v>
+        <v>1.4485863493243201</v>
       </c>
       <c r="N11">
         <f>(N10-P10)/P10*100</f>
-        <v>-9.6865516876268103</v>
+        <v>0.77766697345848823</v>
       </c>
       <c r="P11">
         <f>(P5-P10)/P10*100</f>
-        <v>-1.9902789731007504</v>
+        <v>-60.688204507883917</v>
       </c>
       <c r="R11">
         <f t="shared" ref="R11:R32" si="0">D11/23+2.5</f>
@@ -11625,10 +11629,10 @@
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S32" si="1">E11*3.9+2.5</f>
-        <v>2.672611432486768</v>
-      </c>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
+        <v>3.1680115606657169</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C12">
         <f>2*PI()/10*2</f>
         <v>1.2566370614359172</v>
@@ -11639,11 +11643,11 @@
       </c>
       <c r="E12">
         <f>G5*SIN(C12+H5)</f>
-        <v>6.3170537463956414E-2</v>
+        <v>0.19230450023886728</v>
       </c>
       <c r="G12">
         <f t="shared" ref="G12:G32" si="3">D12*E12/0.282</f>
-        <v>4.2180801008697699</v>
+        <v>12.840729528826595</v>
       </c>
       <c r="R12">
         <f t="shared" si="0"/>
@@ -11651,10 +11655,10 @@
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>2.7463650961094301</v>
-      </c>
-    </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.3">
+        <v>3.2499875509315821</v>
+      </c>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13">
         <f>2*PI()/10*3</f>
         <v>1.8849555921538759</v>
@@ -11665,11 +11669,11 @@
       </c>
       <c r="E13">
         <f>G5*SIN(C13+H5)</f>
-        <v>5.7952735041006211E-2</v>
+        <v>0.13987020202073749</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>3.8696722915635058</v>
+        <v>9.3395392778625332</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
@@ -11677,10 +11681,10 @@
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>2.726015666659924</v>
-      </c>
-    </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
+        <v>3.0454937878808761</v>
+      </c>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>2*PI()/10*4</f>
         <v>2.5132741228718345</v>
@@ -11691,11 +11695,11 @@
       </c>
       <c r="E14">
         <f>G5*SIN(C14+H5)</f>
-        <v>3.0598957573408671E-2</v>
+        <v>3.4010240644000225E-2</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>1.2627554219564039</v>
+        <v>1.4035319887032727</v>
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
@@ -11703,10 +11707,10 @@
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>2.6193359345362937</v>
-      </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
+        <v>2.6326399385116011</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>2*PI()/10*5</f>
         <v>3.1415926535897931</v>
@@ -11717,11 +11721,11 @@
       </c>
       <c r="E15">
         <f>G5*SIN(C15+H5)</f>
-        <v>-8.4425816669149775E-3</v>
+        <v>-8.4840476693182024E-2</v>
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>-7.2620278849267763E-17</v>
+        <v>-7.2976955607170768E-16</v>
       </c>
       <c r="R15">
         <f t="shared" si="0"/>
@@ -11729,10 +11733,10 @@
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>2.4670739314990318</v>
-      </c>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.3">
+        <v>2.1691221408965902</v>
+      </c>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16">
         <f>2*PI()/10*6</f>
         <v>3.7699111843077517</v>
@@ -11743,11 +11747,11 @@
       </c>
       <c r="E16">
         <f>G5*SIN(C16+H5)</f>
-        <v>-4.4259341663273846E-2</v>
+        <v>-0.17128501555531206</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>1.8264910993598296</v>
+        <v>7.0685768158429036</v>
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
@@ -11755,10 +11759,10 @@
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>2.327388567513232</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+        <v>1.8319884393342831</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>2*PI()/10*7</f>
         <v>4.3982297150257104</v>
@@ -11769,11 +11773,11 @@
       </c>
       <c r="E17">
         <f>G5*SIN(C17+H5)</f>
-        <v>-6.3170537463956414E-2</v>
+        <v>-0.19230450023886728</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>4.2180801008697699</v>
+        <v>12.840729528826595</v>
       </c>
       <c r="R17">
         <f t="shared" si="0"/>
@@ -11781,10 +11785,10 @@
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>2.2536349038905699</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
+        <v>1.7500124490684177</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>2*PI()/10*8</f>
         <v>5.026548245743669</v>
@@ -11795,11 +11799,11 @@
       </c>
       <c r="E18">
         <f>G5*SIN(C18+H5)</f>
-        <v>-5.7952735041006218E-2</v>
+        <v>-0.13987020202073747</v>
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>3.8696722915635067</v>
+        <v>9.3395392778625315</v>
       </c>
       <c r="R18">
         <f t="shared" si="0"/>
@@ -11807,10 +11811,10 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>2.273984333340076</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+        <v>1.9545062121191239</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C19">
         <f>2*PI()/10*9</f>
         <v>5.6548667764616276</v>
@@ -11821,11 +11825,11 @@
       </c>
       <c r="E19">
         <f>G5*SIN(C19+H5)</f>
-        <v>-3.0598957573408678E-2</v>
+        <v>-3.401024064400017E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>1.2627554219564043</v>
+        <v>1.4035319887032707</v>
       </c>
       <c r="R19">
         <f t="shared" si="0"/>
@@ -11833,10 +11837,10 @@
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>2.3806640654637063</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+        <v>2.3673600614883994</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C20">
         <f>2*PI()/10*10</f>
         <v>6.2831853071795862</v>
@@ -11847,11 +11851,11 @@
       </c>
       <c r="E20">
         <f>G5*SIN(C20+H5)</f>
-        <v>8.4425816669149688E-3</v>
+        <v>8.4840476693182065E-2</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>-1.4524055769853538E-16</v>
+        <v>-1.4595391121434159E-15</v>
       </c>
       <c r="R20">
         <f t="shared" si="0"/>
@@ -11859,10 +11863,10 @@
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>2.5329260685009682</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+        <v>2.8308778591034098</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C21">
         <f>2*PI()/10*11</f>
         <v>6.9115038378975449</v>
@@ -11873,11 +11877,11 @@
       </c>
       <c r="E21">
         <f>G5*SIN(C21+H5)</f>
-        <v>4.4259341663273846E-2</v>
+        <v>0.17128501555531203</v>
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>1.8264910993598293</v>
+        <v>7.0685768158429019</v>
       </c>
       <c r="R21">
         <f t="shared" si="0"/>
@@ -11885,10 +11889,10 @@
       </c>
       <c r="S21">
         <f t="shared" si="1"/>
-        <v>2.672611432486768</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+        <v>3.1680115606657169</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
@@ -11902,11 +11906,11 @@
       </c>
       <c r="E22">
         <f>G5*SIN(C22+H6)</f>
-        <v>4.275615837630773E-2</v>
+        <v>0.12923086443407317</v>
       </c>
       <c r="G22">
         <f t="shared" si="3"/>
-        <v>1.9980951366638227</v>
+        <v>6.0392601098527861</v>
       </c>
       <c r="R22">
         <f t="shared" si="0"/>
@@ -11914,10 +11918,10 @@
       </c>
       <c r="S22">
         <f t="shared" si="1"/>
-        <v>2.6667490176676001</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+        <v>3.0040003712928853</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <f>0.1</f>
         <v>0.1</v>
@@ -11932,11 +11936,11 @@
       </c>
       <c r="E23">
         <f>G5*SIN(C23+H5)</f>
-        <v>6.4017837101842542E-2</v>
+        <v>0.18867592669967226</v>
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
-        <v>4.3919619243204684</v>
+        <v>12.944165620318811</v>
       </c>
       <c r="R23">
         <f t="shared" si="0"/>
@@ -11944,10 +11948,10 @@
       </c>
       <c r="S23">
         <f t="shared" si="1"/>
-        <v>2.7496695646971858</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+        <v>3.2358361141287215</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C24">
         <f>C13+B25</f>
         <v>1.8849555921538759</v>
@@ -11958,11 +11962,11 @@
       </c>
       <c r="E24">
         <f>G5*SIN(C24+H5)</f>
-        <v>5.7952735041006211E-2</v>
+        <v>0.13987020202073749</v>
       </c>
       <c r="G24">
         <f t="shared" si="3"/>
-        <v>3.8696722915635058</v>
+        <v>9.3395392778625332</v>
       </c>
       <c r="R24">
         <f t="shared" si="0"/>
@@ -11970,10 +11974,10 @@
       </c>
       <c r="S24">
         <f t="shared" si="1"/>
-        <v>2.726015666659924</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+        <v>3.0454937878808761</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C25">
         <f>C14+B23</f>
         <v>2.6132741228718346</v>
@@ -11984,11 +11988,11 @@
       </c>
       <c r="E25">
         <f>G5*SIN(C25+H5)</f>
-        <v>2.4807575755358302E-2</v>
+        <v>1.475714151490275E-2</v>
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>0.87796925203578624</v>
+        <v>0.52227257615959999</v>
       </c>
       <c r="R25">
         <f t="shared" si="0"/>
@@ -11996,10 +12000,10 @@
       </c>
       <c r="S25">
         <f t="shared" si="1"/>
-        <v>2.5967495454458973</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+        <v>2.5575528519081208</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>C15+B23</f>
         <v>3.2415926535897932</v>
@@ -12010,11 +12014,11 @@
       </c>
       <c r="E26">
         <f>G5*SIN(C26+H5)</f>
-        <v>-1.4757623459834451E-2</v>
+        <v>-0.10185099404437847</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>0.10343946955157717</v>
+        <v>0.71389630084582323</v>
       </c>
       <c r="R26">
         <f t="shared" si="0"/>
@@ -12022,10 +12026,10 @@
       </c>
       <c r="S26">
         <f t="shared" si="1"/>
-        <v>2.4424452685066456</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+        <v>2.102781123226924</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>C16+B23</f>
         <v>3.8699111843077518</v>
@@ -12036,11 +12040,11 @@
       </c>
       <c r="E27">
         <f>G5*SIN(C27+H5)</f>
-        <v>-4.8685912106543244E-2</v>
+        <v>-0.17955551166667025</v>
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
-        <v>2.2752063772415805</v>
+        <v>8.3910484067521161</v>
       </c>
       <c r="R27">
         <f t="shared" si="0"/>
@@ -12048,10 +12052,10 @@
       </c>
       <c r="S27">
         <f t="shared" si="1"/>
-        <v>2.3101249427844812</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+        <v>1.799733504499986</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C28">
         <f>C17+B23</f>
         <v>4.49822971502571</v>
@@ -12062,11 +12066,11 @@
       </c>
       <c r="E28">
         <f>G5*SIN(C28+H5)</f>
-        <v>-6.4017837101842542E-2</v>
+        <v>-0.18867592669967229</v>
       </c>
       <c r="G28">
         <f t="shared" si="3"/>
-        <v>4.3919619243204684</v>
+        <v>12.944165620318813</v>
       </c>
       <c r="R28">
         <f t="shared" si="0"/>
@@ -12074,10 +12078,10 @@
       </c>
       <c r="S28">
         <f t="shared" si="1"/>
-        <v>2.2503304353028142</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
+        <v>1.764163885871278</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>C18+B23</f>
         <v>5.1265482457436686</v>
@@ -12088,11 +12092,11 @@
       </c>
       <c r="E29">
         <f>G5*SIN(C29+H5)</f>
-        <v>-5.4897124210492046E-2</v>
+        <v>-0.12572855059228327</v>
       </c>
       <c r="G29">
         <f t="shared" si="3"/>
-        <v>3.528421890600097</v>
+        <v>8.0809947071589576</v>
       </c>
       <c r="R29">
         <f t="shared" si="0"/>
@@ -12100,10 +12104,10 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>2.2859012155790812</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
+        <v>2.0096586526900952</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C30">
         <f>C19+B23</f>
         <v>5.7548667764616273</v>
@@ -12114,11 +12118,11 @@
       </c>
       <c r="E30">
         <f>G5*SIN(C30+H5)</f>
-        <v>-2.4807575755358337E-2</v>
+        <v>-1.4757141514902775E-2</v>
       </c>
       <c r="G30">
         <f t="shared" si="3"/>
-        <v>0.87796925203578857</v>
+        <v>0.52227257615960165</v>
       </c>
       <c r="R30">
         <f t="shared" si="0"/>
@@ -12126,10 +12130,10 @@
       </c>
       <c r="S30">
         <f t="shared" si="1"/>
-        <v>2.4032504545541027</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+        <v>2.4424471480918792</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C31">
         <f>C20+B23</f>
         <v>6.3831853071795859</v>
@@ -12140,11 +12144,11 @@
       </c>
       <c r="E31">
         <f>G5*SIN(C31+H5)</f>
-        <v>1.4757623459834415E-2</v>
+        <v>0.10185099404437847</v>
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
-        <v>0.10343946955157633</v>
+        <v>0.71389630084581923</v>
       </c>
       <c r="R31">
         <f t="shared" si="0"/>
@@ -12152,10 +12156,10 @@
       </c>
       <c r="S31">
         <f t="shared" si="1"/>
-        <v>2.5575547314933544</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
+        <v>2.897218876773076</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C32">
         <f>C21+B23</f>
         <v>7.0115038378975445</v>
@@ -12166,11 +12170,11 @@
       </c>
       <c r="E32">
         <f>G5*SIN(C32+H5)</f>
-        <v>4.8685912106543237E-2</v>
+        <v>0.17955551166667025</v>
       </c>
       <c r="G32">
         <f t="shared" si="3"/>
-        <v>2.2752063772415787</v>
+        <v>8.3910484067521089</v>
       </c>
       <c r="R32">
         <f t="shared" si="0"/>
@@ -12178,10 +12182,10 @@
       </c>
       <c r="S32">
         <f t="shared" si="1"/>
-        <v>2.6898750572155188</v>
-      </c>
-    </row>
-    <row r="35" spans="3:24" x14ac:dyDescent="0.3">
+        <v>3.200266495500014</v>
+      </c>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.25">
       <c r="K35" t="s">
         <v>333</v>
       </c>
@@ -12201,7 +12205,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="36" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:24" x14ac:dyDescent="0.25">
       <c r="V36" t="s">
         <v>340</v>
       </c>
@@ -12209,7 +12213,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="37" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>26</v>
       </c>
@@ -12269,7 +12273,7 @@
         <v>0.64820024095290063</v>
       </c>
     </row>
-    <row r="38" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>28</v>
       </c>
@@ -12310,29 +12314,29 @@
       </c>
       <c r="S38">
         <f>(S37-P10)/P10*100</f>
-        <v>138.87795511675887</v>
+        <v>-4.1858172767619539</v>
       </c>
       <c r="T38">
         <f>(T37-P10)/P10*100</f>
-        <v>207.28482416649743</v>
+        <v>23.252245174219045</v>
       </c>
       <c r="U38" t="s">
         <v>336</v>
       </c>
       <c r="V38">
         <f>(V37-14)/C3*100</f>
-        <v>-6.1978386165852592E-2</v>
+        <v>-6.8176224782437858E-2</v>
       </c>
       <c r="W38">
         <f>(W37-F5)/F5*100</f>
-        <v>194.42586772614683</v>
+        <v>-2.5889125967816176</v>
       </c>
       <c r="X38">
         <f>(X37-F5*SQRT(2))/(F5*SQRT(2))*100</f>
-        <v>184.56611174090779</v>
-      </c>
-    </row>
-    <row r="39" spans="3:24" x14ac:dyDescent="0.3">
+        <v>-5.8510225447630555</v>
+      </c>
+    </row>
+    <row r="39" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>30</v>
       </c>
@@ -12372,7 +12376,7 @@
         <v>12.248662368322119</v>
       </c>
     </row>
-    <row r="40" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>31</v>
       </c>
@@ -12412,7 +12416,7 @@
         <v>8.7479761154527225</v>
       </c>
     </row>
-    <row r="41" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>32</v>
       </c>
@@ -12452,7 +12456,7 @@
         <v>1.1128801761009104</v>
       </c>
     </row>
-    <row r="42" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>33</v>
       </c>
@@ -12492,7 +12496,7 @@
         <v>-0.16553594017271608</v>
       </c>
     </row>
-    <row r="43" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>34</v>
       </c>
@@ -12532,7 +12536,7 @@
         <v>6.6962279413240271</v>
       </c>
     </row>
-    <row r="44" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>35</v>
       </c>
@@ -12572,7 +12576,7 @@
         <v>12.248662368322119</v>
       </c>
     </row>
-    <row r="45" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>37</v>
       </c>
@@ -12612,7 +12616,7 @@
         <v>8.8202734387209265</v>
       </c>
     </row>
-    <row r="46" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>39</v>
       </c>
@@ -12652,7 +12656,7 @@
         <v>1.1128801761009104</v>
       </c>
     </row>
-    <row r="47" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>41</v>
       </c>
@@ -12692,7 +12696,7 @@
         <v>-0.16553594017271608</v>
       </c>
     </row>
-    <row r="48" spans="3:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>42</v>
       </c>
@@ -12732,7 +12736,7 @@
         <v>6.7386091308260783</v>
       </c>
     </row>
-    <row r="49" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>43</v>
       </c>
@@ -12772,7 +12776,7 @@
         <v>12.248662368322119</v>
       </c>
     </row>
-    <row r="50" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>44</v>
       </c>
@@ -12812,7 +12816,7 @@
         <v>8.8202734387209265</v>
       </c>
     </row>
-    <row r="51" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>45</v>
       </c>
@@ -12852,7 +12856,7 @@
         <v>1.1128801761009104</v>
       </c>
     </row>
-    <row r="52" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>46</v>
       </c>
@@ -12892,7 +12896,7 @@
         <v>-0.16553594017271608</v>
       </c>
     </row>
-    <row r="53" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>48</v>
       </c>
@@ -12932,7 +12936,7 @@
         <v>6.6962279413240271</v>
       </c>
     </row>
-    <row r="54" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>50</v>
       </c>
@@ -12972,7 +12976,7 @@
         <v>12.248662368322119</v>
       </c>
     </row>
-    <row r="55" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>52</v>
       </c>
@@ -13012,7 +13016,7 @@
         <v>8.8202734387209265</v>
       </c>
     </row>
-    <row r="56" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>53</v>
       </c>
@@ -13052,7 +13056,7 @@
         <v>1.1128801761009104</v>
       </c>
     </row>
-    <row r="57" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>54</v>
       </c>
@@ -13092,7 +13096,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="58" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>55</v>
       </c>
@@ -13132,7 +13136,7 @@
         <v>6.4419408043117228</v>
       </c>
     </row>
-    <row r="59" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>56</v>
       </c>
@@ -13173,7 +13177,7 @@
       </c>
       <c r="AD59" s="2"/>
     </row>
-    <row r="60" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>57</v>
       </c>
@@ -13218,7 +13222,7 @@
       </c>
       <c r="AD60" s="2"/>
     </row>
-    <row r="61" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>59</v>
       </c>
@@ -13259,7 +13263,7 @@
       </c>
       <c r="AD61" s="2"/>
     </row>
-    <row r="62" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>61</v>
       </c>
@@ -13300,7 +13304,7 @@
       </c>
       <c r="AD62" s="2"/>
     </row>
-    <row r="63" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>63</v>
       </c>
@@ -13341,7 +13345,7 @@
       </c>
       <c r="AD63" s="2"/>
     </row>
-    <row r="64" spans="3:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>64</v>
       </c>
@@ -13381,7 +13385,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="65" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>65</v>
       </c>
@@ -13421,7 +13425,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="66" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>66</v>
       </c>
@@ -13461,7 +13465,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="67" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>67</v>
       </c>
@@ -13501,7 +13505,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="68" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>68</v>
       </c>
@@ -13541,7 +13545,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="69" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>70</v>
       </c>
@@ -13581,7 +13585,7 @@
         <v>12.477520791633193</v>
       </c>
     </row>
-    <row r="70" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>72</v>
       </c>
@@ -13621,7 +13625,7 @@
         <v>9.5362662401908675</v>
       </c>
     </row>
-    <row r="71" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>74</v>
       </c>
@@ -13661,7 +13665,7 @@
         <v>1.7156902714889037</v>
       </c>
     </row>
-    <row r="72" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>76</v>
       </c>
@@ -13701,7 +13705,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="73" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>78</v>
       </c>
@@ -13741,7 +13745,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="74" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>80</v>
       </c>
@@ -13781,7 +13785,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="75" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>82</v>
       </c>
@@ -13821,7 +13825,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="76" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>84</v>
       </c>
@@ -13861,7 +13865,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="77" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>86</v>
       </c>
@@ -13901,7 +13905,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="78" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>88</v>
       </c>
@@ -13941,7 +13945,7 @@
         <v>6.4419408043117228</v>
       </c>
     </row>
-    <row r="79" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>90</v>
       </c>
@@ -13981,7 +13985,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="80" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>92</v>
       </c>
@@ -14021,7 +14025,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>94</v>
       </c>
@@ -14061,7 +14065,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>96</v>
       </c>
@@ -14101,7 +14105,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="83" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>98</v>
       </c>
@@ -14141,7 +14145,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="84" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>100</v>
       </c>
@@ -14181,7 +14185,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="85" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>102</v>
       </c>
@@ -14221,7 +14225,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
         <v>104</v>
       </c>
@@ -14261,7 +14265,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>106</v>
       </c>
@@ -14301,7 +14305,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="88" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>108</v>
       </c>
@@ -14341,7 +14345,7 @@
         <v>6.4419408043117228</v>
       </c>
     </row>
-    <row r="89" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
         <v>110</v>
       </c>
@@ -14381,7 +14385,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="90" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>112</v>
       </c>
@@ -14421,7 +14425,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
         <v>114</v>
       </c>
@@ -14461,7 +14465,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="92" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>116</v>
       </c>
@@ -14501,7 +14505,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="93" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>118</v>
       </c>
@@ -14541,7 +14545,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="94" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>120</v>
       </c>
@@ -14581,7 +14585,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="95" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>122</v>
       </c>
@@ -14621,7 +14625,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="96" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
         <v>124</v>
       </c>
@@ -14661,7 +14665,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="97" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>126</v>
       </c>
@@ -14701,7 +14705,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="98" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
         <v>128</v>
       </c>
@@ -14741,7 +14745,7 @@
         <v>6.4419408043117228</v>
       </c>
     </row>
-    <row r="99" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>130</v>
       </c>
@@ -14781,7 +14785,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="100" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
         <v>132</v>
       </c>
@@ -14821,7 +14825,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="101" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
         <v>134</v>
       </c>
@@ -14861,7 +14865,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="102" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
         <v>136</v>
       </c>
@@ -14901,7 +14905,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="103" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
         <v>138</v>
       </c>
@@ -14941,7 +14945,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="104" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
         <v>139</v>
       </c>
@@ -14981,7 +14985,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="105" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
         <v>140</v>
       </c>
@@ -15021,7 +15025,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="106" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
         <v>141</v>
       </c>
@@ -15061,7 +15065,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="107" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
         <v>142</v>
       </c>
@@ -15101,7 +15105,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="108" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
         <v>143</v>
       </c>
@@ -15141,7 +15145,7 @@
         <v>6.4419408043117228</v>
       </c>
     </row>
-    <row r="109" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
         <v>145</v>
       </c>
@@ -15181,7 +15185,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="110" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
         <v>147</v>
       </c>
@@ -15221,7 +15225,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="111" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
         <v>149</v>
       </c>
@@ -15261,7 +15265,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="112" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
         <v>151</v>
       </c>
@@ -15301,7 +15305,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="113" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
         <v>153</v>
       </c>
@@ -15341,7 +15345,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="114" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
         <v>155</v>
       </c>
@@ -15381,7 +15385,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="115" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
         <v>157</v>
       </c>
@@ -15421,7 +15425,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="116" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
         <v>159</v>
       </c>
@@ -15461,7 +15465,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="117" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
         <v>161</v>
       </c>
@@ -15501,7 +15505,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="118" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
         <v>163</v>
       </c>
@@ -15541,7 +15545,7 @@
         <v>6.4419408043117228</v>
       </c>
     </row>
-    <row r="119" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
         <v>165</v>
       </c>
@@ -15581,7 +15585,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="120" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
         <v>166</v>
       </c>
@@ -15621,7 +15625,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="121" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
         <v>167</v>
       </c>
@@ -15661,7 +15665,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="122" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
         <v>168</v>
       </c>
@@ -15701,7 +15705,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="123" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
         <v>169</v>
       </c>
@@ -15741,7 +15745,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="124" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
         <v>170</v>
       </c>
@@ -15781,7 +15785,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="125" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
         <v>172</v>
       </c>
@@ -15821,7 +15825,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="126" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
         <v>174</v>
       </c>
@@ -15861,7 +15865,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="127" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
         <v>176</v>
       </c>
@@ -15901,7 +15905,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="128" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
         <v>177</v>
       </c>
@@ -15941,7 +15945,7 @@
         <v>6.4419408043117228</v>
       </c>
     </row>
-    <row r="129" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
         <v>178</v>
       </c>
@@ -15981,7 +15985,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="130" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
         <v>179</v>
       </c>
@@ -16021,7 +16025,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="131" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
         <v>180</v>
       </c>
@@ -16061,7 +16065,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="132" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
         <v>181</v>
       </c>
@@ -16101,7 +16105,7 @@
         <v>-0.14160303315979328</v>
       </c>
     </row>
-    <row r="133" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C133" t="s">
         <v>182</v>
       </c>
@@ -16141,7 +16145,7 @@
         <v>6.5177283431859783</v>
       </c>
     </row>
-    <row r="134" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C134" t="s">
         <v>183</v>
       </c>
@@ -16181,7 +16185,7 @@
         <v>12.39026540148191</v>
       </c>
     </row>
-    <row r="135" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
         <v>184</v>
       </c>
@@ -16221,7 +16225,7 @@
         <v>9.4709493481347646</v>
       </c>
     </row>
-    <row r="136" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
         <v>185</v>
       </c>
@@ -16261,7 +16265,7 @@
         <v>1.6972419889997756</v>
       </c>
     </row>
-    <row r="137" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
         <v>186</v>
       </c>
@@ -16303,6 +16307,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>